<commit_message>
feat: add positions order form file
</commit_message>
<xml_diff>
--- a/server/orders/OrderFormTmpEng.xlsx
+++ b/server/orders/OrderFormTmpEng.xlsx
@@ -139,9 +139,6 @@
     <t>SWS (std)</t>
   </si>
   <si>
-    <t>Fire2 (std)</t>
-  </si>
-  <si>
     <t>Demon (std)</t>
   </si>
   <si>
@@ -429,6 +426,9 @@
   </si>
   <si>
     <t>FIRE1 rev. 06.2021</t>
+  </si>
+  <si>
+    <t>Fire (std)</t>
   </si>
 </sst>
 </file>
@@ -864,66 +864,153 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -938,140 +1025,53 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1797,8 +1797,8 @@
   </sheetPr>
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="AH60" sqref="AH60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1810,35 +1810,35 @@
   <sheetData>
     <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="99" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-      <c r="F1" s="99"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="94" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="94"/>
-      <c r="M1" s="94"/>
-      <c r="N1" s="94"/>
-      <c r="O1" s="94"/>
-      <c r="P1" s="94"/>
-      <c r="Q1" s="94"/>
-      <c r="R1" s="94"/>
-      <c r="S1" s="94"/>
-      <c r="T1" s="94"/>
-      <c r="U1" s="94"/>
-      <c r="V1" s="94"/>
-      <c r="W1" s="94"/>
-      <c r="X1" s="94"/>
-      <c r="Y1" s="94"/>
-      <c r="Z1" s="94"/>
+      <c r="B1" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="105" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="105"/>
+      <c r="R1" s="105"/>
+      <c r="S1" s="105"/>
+      <c r="T1" s="105"/>
+      <c r="U1" s="105"/>
+      <c r="V1" s="105"/>
+      <c r="W1" s="105"/>
+      <c r="X1" s="105"/>
+      <c r="Y1" s="105"/>
+      <c r="Z1" s="105"/>
       <c r="AA1" s="8"/>
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
@@ -1848,31 +1848,31 @@
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="94"/>
-      <c r="T2" s="94"/>
-      <c r="U2" s="94"/>
-      <c r="V2" s="94"/>
-      <c r="W2" s="94"/>
-      <c r="X2" s="94"/>
-      <c r="Y2" s="94"/>
-      <c r="Z2" s="94"/>
+      <c r="B2" s="106"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="106"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
@@ -1882,31 +1882,31 @@
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
-      <c r="T3" s="94"/>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="94"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
+      <c r="F3" s="106"/>
+      <c r="G3" s="106"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="105"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105"/>
+      <c r="V3" s="105"/>
+      <c r="W3" s="105"/>
+      <c r="X3" s="105"/>
+      <c r="Y3" s="105"/>
+      <c r="Z3" s="105"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
@@ -1915,70 +1915,70 @@
       <c r="AF3" s="8"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="81"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="107" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="68"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="68"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="110"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A8" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="68"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="81"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="100" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="81"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="103"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="81"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="71" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="72"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -1987,10 +1987,10 @@
       <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="72"/>
+      <c r="A10" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="67"/>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
@@ -1999,10 +1999,10 @@
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="72"/>
+      <c r="A11" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="67"/>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -2011,10 +2011,10 @@
       <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="72"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -2023,10 +2023,10 @@
       <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A13" s="92" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="92"/>
+      <c r="A13" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="112"/>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
@@ -2035,65 +2035,65 @@
       <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A14" s="71" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
+      <c r="A14" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
       <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A15" s="90" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="91"/>
+      <c r="A15" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="111"/>
       <c r="E15" s="38"/>
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
       <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" s="82" t="s">
+      <c r="A16" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="67"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A17" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="81"/>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A17" s="71" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A18" s="93" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="93"/>
+      <c r="A18" s="113" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="113"/>
       <c r="C18" s="36"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="71" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
+      <c r="E18" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="2"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -2121,17 +2121,17 @@
       <c r="AF18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="93" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="93"/>
+      <c r="A19" s="113" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="113"/>
       <c r="C19" s="36"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="71" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="E19" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="2"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
@@ -2159,166 +2159,166 @@
       <c r="AF19" s="13"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="93"/>
+      <c r="A20" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="113"/>
       <c r="C20" s="36"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="E20" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="95" t="s">
-        <v>84</v>
-      </c>
-      <c r="J20" s="96"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96"/>
-      <c r="T20" s="97"/>
-      <c r="U20" s="95" t="s">
-        <v>113</v>
-      </c>
-      <c r="V20" s="96"/>
-      <c r="W20" s="96"/>
-      <c r="X20" s="96"/>
-      <c r="Y20" s="96"/>
-      <c r="Z20" s="96"/>
-      <c r="AA20" s="96"/>
-      <c r="AB20" s="96"/>
-      <c r="AC20" s="96"/>
-      <c r="AD20" s="96"/>
-      <c r="AE20" s="96"/>
-      <c r="AF20" s="96"/>
+      <c r="I20" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="77"/>
+      <c r="U20" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="V20" s="63"/>
+      <c r="W20" s="63"/>
+      <c r="X20" s="63"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="63"/>
+      <c r="AA20" s="63"/>
+      <c r="AB20" s="63"/>
+      <c r="AC20" s="63"/>
+      <c r="AD20" s="63"/>
+      <c r="AE20" s="63"/>
+      <c r="AF20" s="63"/>
     </row>
     <row r="21" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="93" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="93"/>
+      <c r="A21" s="113" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="113"/>
       <c r="C21" s="36"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
+      <c r="E21" s="69" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="95" t="s">
-        <v>85</v>
-      </c>
-      <c r="J21" s="96"/>
-      <c r="K21" s="96"/>
-      <c r="L21" s="96"/>
-      <c r="M21" s="96"/>
-      <c r="N21" s="96"/>
-      <c r="O21" s="96"/>
-      <c r="P21" s="96"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="97"/>
-      <c r="U21" s="88" t="s">
+      <c r="I21" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="77"/>
+      <c r="U21" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="V21" s="89"/>
-      <c r="W21" s="89"/>
+      <c r="V21" s="65"/>
+      <c r="W21" s="65"/>
       <c r="X21" s="35"/>
-      <c r="Y21" s="89" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="89"/>
+      <c r="Y21" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z21" s="65"/>
+      <c r="AA21" s="65"/>
       <c r="AB21" s="35"/>
-      <c r="AC21" s="98" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD21" s="98"/>
-      <c r="AE21" s="98"/>
+      <c r="AC21" s="97" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD21" s="97"/>
+      <c r="AE21" s="97"/>
       <c r="AF21" s="35"/>
     </row>
     <row r="22" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="93" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="93"/>
+      <c r="A22" s="113" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="113"/>
       <c r="C22" s="36"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="71" t="s">
-        <v>63</v>
-      </c>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
+      <c r="E22" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="88" t="s">
+      <c r="I22" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="89"/>
-      <c r="K22" s="89"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
       <c r="L22" s="35"/>
-      <c r="M22" s="89" t="s">
+      <c r="M22" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="89"/>
-      <c r="O22" s="89"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
       <c r="P22" s="35"/>
-      <c r="Q22" s="89" t="s">
+      <c r="Q22" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="R22" s="89"/>
-      <c r="S22" s="89"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
       <c r="T22" s="34"/>
-      <c r="U22" s="88" t="s">
+      <c r="U22" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="V22" s="65"/>
+      <c r="W22" s="65"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="V22" s="89"/>
-      <c r="W22" s="89"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="Z22" s="89"/>
-      <c r="AA22" s="89"/>
-      <c r="AB22" s="89"/>
-      <c r="AC22" s="89"/>
+      <c r="Z22" s="65"/>
+      <c r="AA22" s="65"/>
+      <c r="AB22" s="65"/>
+      <c r="AC22" s="65"/>
       <c r="AD22" s="56"/>
       <c r="AE22" s="56"/>
       <c r="AF22" s="56"/>
     </row>
     <row r="23" spans="1:33" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="82"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="83"/>
-      <c r="I23" s="95" t="s">
-        <v>86</v>
-      </c>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96"/>
-      <c r="T23" s="97"/>
+        <v>63</v>
+      </c>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="114"/>
+      <c r="I23" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="77"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
       <c r="W23" s="13"/>
@@ -2327,173 +2327,173 @@
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
-      <c r="AC23" s="107" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD23" s="107"/>
-      <c r="AE23" s="107"/>
-      <c r="AF23" s="108"/>
+      <c r="AC23" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD23" s="71"/>
+      <c r="AE23" s="71"/>
+      <c r="AF23" s="72"/>
       <c r="AG23" s="19"/>
     </row>
     <row r="24" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="84" t="s">
+      <c r="D24" s="116"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="85"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="84" t="s">
+      <c r="G24" s="115"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="95"/>
+      <c r="K24" s="95"/>
+      <c r="L24" s="95"/>
+      <c r="M24" s="95"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="65"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="V24" s="63"/>
+      <c r="W24" s="63"/>
+      <c r="X24" s="63"/>
+      <c r="Y24" s="63"/>
+      <c r="Z24" s="63"/>
+      <c r="AA24" s="63"/>
+      <c r="AB24" s="63"/>
+      <c r="AC24" s="63"/>
+      <c r="AD24" s="63"/>
+      <c r="AE24" s="63"/>
+      <c r="AF24" s="63"/>
+    </row>
+    <row r="25" spans="1:33" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="84"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="88" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="P24" s="89"/>
-      <c r="Q24" s="89"/>
-      <c r="R24" s="89"/>
-      <c r="S24" s="89"/>
-      <c r="T24" s="54"/>
-      <c r="U24" s="95" t="s">
-        <v>118</v>
-      </c>
-      <c r="V24" s="96"/>
-      <c r="W24" s="96"/>
-      <c r="X24" s="96"/>
-      <c r="Y24" s="96"/>
-      <c r="Z24" s="96"/>
-      <c r="AA24" s="96"/>
-      <c r="AB24" s="96"/>
-      <c r="AC24" s="96"/>
-      <c r="AD24" s="96"/>
-      <c r="AE24" s="96"/>
-      <c r="AF24" s="96"/>
-    </row>
-    <row r="25" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
       <c r="G25" s="36"/>
       <c r="H25" s="42"/>
-      <c r="I25" s="95" t="s">
-        <v>64</v>
-      </c>
-      <c r="J25" s="96"/>
-      <c r="K25" s="96"/>
-      <c r="L25" s="96"/>
-      <c r="M25" s="96"/>
-      <c r="N25" s="96"/>
-      <c r="O25" s="96"/>
-      <c r="P25" s="96"/>
-      <c r="Q25" s="96"/>
-      <c r="R25" s="96"/>
-      <c r="S25" s="96"/>
-      <c r="T25" s="97"/>
-      <c r="U25" s="88" t="s">
+      <c r="I25" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="77"/>
+      <c r="U25" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="V25" s="89"/>
-      <c r="W25" s="89"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="65"/>
       <c r="X25" s="35"/>
-      <c r="Y25" s="89" t="s">
+      <c r="Y25" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="Z25" s="89"/>
-      <c r="AA25" s="89"/>
+      <c r="Z25" s="65"/>
+      <c r="AA25" s="65"/>
       <c r="AB25" s="35"/>
-      <c r="AC25" s="89" t="s">
+      <c r="AC25" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="AD25" s="89"/>
-      <c r="AE25" s="89"/>
+      <c r="AD25" s="65"/>
+      <c r="AE25" s="65"/>
       <c r="AF25" s="35"/>
     </row>
     <row r="26" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="71" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
+      <c r="A26" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="67"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="42"/>
       <c r="I26" s="104" t="s">
+        <v>87</v>
+      </c>
+      <c r="J26" s="80"/>
+      <c r="K26" s="80"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="J26" s="105"/>
-      <c r="K26" s="105"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="106" t="s">
-        <v>89</v>
-      </c>
-      <c r="N26" s="106"/>
-      <c r="O26" s="106"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
       <c r="P26" s="35"/>
-      <c r="Q26" s="89" t="s">
+      <c r="Q26" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="R26" s="89"/>
-      <c r="S26" s="89"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
       <c r="T26" s="34"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
       <c r="X26" s="13"/>
-      <c r="Y26" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="89"/>
-      <c r="AB26" s="89"/>
-      <c r="AC26" s="89"/>
+      <c r="Y26" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z26" s="65"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
       <c r="AD26" s="56"/>
       <c r="AE26" s="56"/>
       <c r="AF26" s="56"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="82"/>
+        <v>69</v>
+      </c>
+      <c r="B27" s="66"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="95" t="s">
-        <v>90</v>
-      </c>
-      <c r="J27" s="96"/>
-      <c r="K27" s="96"/>
-      <c r="L27" s="96"/>
-      <c r="M27" s="96"/>
-      <c r="N27" s="96"/>
-      <c r="O27" s="96"/>
-      <c r="P27" s="96"/>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="S27" s="96"/>
-      <c r="T27" s="97"/>
+      <c r="I27" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="63"/>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="77"/>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
       <c r="W27" s="13"/>
@@ -2502,144 +2502,144 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="13"/>
-      <c r="AC27" s="107" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD27" s="107"/>
-      <c r="AE27" s="107"/>
-      <c r="AF27" s="108"/>
+      <c r="AC27" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD27" s="71"/>
+      <c r="AE27" s="71"/>
+      <c r="AF27" s="72"/>
     </row>
     <row r="28" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="31"/>
+      <c r="C28" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="86" t="s">
+      <c r="D28" s="118"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="87"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="86" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="86"/>
+      <c r="G28" s="117"/>
       <c r="H28" s="32"/>
-      <c r="I28" s="88" t="s">
+      <c r="I28" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="65"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="89" t="s">
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="V28" s="63"/>
+      <c r="W28" s="63"/>
+      <c r="X28" s="63"/>
+      <c r="Y28" s="63"/>
+      <c r="Z28" s="63"/>
+      <c r="AA28" s="63"/>
+      <c r="AB28" s="63"/>
+      <c r="AC28" s="63"/>
+      <c r="AD28" s="63"/>
+      <c r="AE28" s="63"/>
+      <c r="AF28" s="63"/>
+    </row>
+    <row r="29" spans="1:33" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="63"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="V29" s="65"/>
+      <c r="W29" s="65"/>
+      <c r="X29" s="35"/>
+      <c r="Y29" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z29" s="65"/>
+      <c r="AA29" s="65"/>
+      <c r="AB29" s="65"/>
+      <c r="AC29" s="35"/>
+      <c r="AD29" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE29" s="65"/>
+      <c r="AF29" s="35"/>
+    </row>
+    <row r="30" spans="1:33" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="89"/>
-      <c r="R28" s="89"/>
-      <c r="S28" s="89"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="95" t="s">
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="65"/>
+      <c r="S30" s="65"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="V28" s="96"/>
-      <c r="W28" s="96"/>
-      <c r="X28" s="96"/>
-      <c r="Y28" s="96"/>
-      <c r="Z28" s="96"/>
-      <c r="AA28" s="96"/>
-      <c r="AB28" s="96"/>
-      <c r="AC28" s="96"/>
-      <c r="AD28" s="96"/>
-      <c r="AE28" s="96"/>
-      <c r="AF28" s="96"/>
-    </row>
-    <row r="29" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="J29" s="96"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="96"/>
-      <c r="T29" s="97"/>
-      <c r="U29" s="88" t="s">
-        <v>24</v>
-      </c>
-      <c r="V29" s="89"/>
-      <c r="W29" s="89"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="89" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z29" s="89"/>
-      <c r="AA29" s="89"/>
-      <c r="AB29" s="89"/>
-      <c r="AC29" s="35"/>
-      <c r="AD29" s="89" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE29" s="89"/>
-      <c r="AF29" s="35"/>
-    </row>
-    <row r="30" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="82" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="88" t="s">
-        <v>93</v>
-      </c>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-      <c r="M30" s="89"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="89" t="s">
-        <v>94</v>
-      </c>
-      <c r="P30" s="89"/>
-      <c r="Q30" s="89"/>
-      <c r="R30" s="89"/>
-      <c r="S30" s="89"/>
-      <c r="T30" s="34"/>
-      <c r="U30" s="95" t="s">
-        <v>120</v>
-      </c>
-      <c r="V30" s="96"/>
-      <c r="W30" s="96"/>
-      <c r="X30" s="96"/>
-      <c r="Y30" s="96"/>
-      <c r="Z30" s="96"/>
-      <c r="AA30" s="96"/>
-      <c r="AB30" s="96"/>
-      <c r="AC30" s="96"/>
-      <c r="AD30" s="96"/>
-      <c r="AE30" s="96"/>
-      <c r="AF30" s="96"/>
+      <c r="V30" s="63"/>
+      <c r="W30" s="63"/>
+      <c r="X30" s="63"/>
+      <c r="Y30" s="63"/>
+      <c r="Z30" s="63"/>
+      <c r="AA30" s="63"/>
+      <c r="AB30" s="63"/>
+      <c r="AC30" s="63"/>
+      <c r="AD30" s="63"/>
+      <c r="AE30" s="63"/>
+      <c r="AF30" s="63"/>
     </row>
     <row r="31" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
@@ -2654,37 +2654,37 @@
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="95" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="96"/>
-      <c r="O31" s="96"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="97"/>
-      <c r="U31" s="134" t="s">
-        <v>121</v>
-      </c>
-      <c r="V31" s="113"/>
-      <c r="W31" s="113"/>
+      <c r="I31" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="63"/>
+      <c r="K31" s="63"/>
+      <c r="L31" s="63"/>
+      <c r="M31" s="63"/>
+      <c r="N31" s="63"/>
+      <c r="O31" s="63"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="63"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="63"/>
+      <c r="T31" s="77"/>
+      <c r="U31" s="103" t="s">
+        <v>120</v>
+      </c>
+      <c r="V31" s="100"/>
+      <c r="W31" s="100"/>
       <c r="X31" s="35"/>
-      <c r="Y31" s="105" t="s">
+      <c r="Y31" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="105"/>
-      <c r="AA31" s="105"/>
+      <c r="Z31" s="80"/>
+      <c r="AA31" s="80"/>
       <c r="AB31" s="35"/>
-      <c r="AC31" s="105" t="s">
+      <c r="AC31" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="AD31" s="105"/>
-      <c r="AE31" s="105"/>
+      <c r="AD31" s="80"/>
+      <c r="AE31" s="80"/>
       <c r="AF31" s="35"/>
     </row>
     <row r="32" spans="1:33" ht="15" x14ac:dyDescent="0.2">
@@ -2700,21 +2700,21 @@
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
       <c r="H32" s="42"/>
-      <c r="I32" s="88" t="s">
+      <c r="I32" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="89"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="89" t="s">
-        <v>92</v>
-      </c>
-      <c r="P32" s="89"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="89"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="65"/>
+      <c r="S32" s="65"/>
       <c r="T32" s="34"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
@@ -2742,20 +2742,20 @@
       <c r="F33" s="36"/>
       <c r="G33" s="36"/>
       <c r="H33" s="42"/>
-      <c r="I33" s="95" t="s">
+      <c r="I33" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="J33" s="96"/>
-      <c r="K33" s="96"/>
-      <c r="L33" s="96"/>
-      <c r="M33" s="96"/>
-      <c r="N33" s="96"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="96"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="97"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="77"/>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
       <c r="W33" s="13"/>
@@ -2782,38 +2782,38 @@
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
       <c r="H34" s="42"/>
-      <c r="I34" s="111" t="s">
+      <c r="I34" s="98" t="s">
+        <v>95</v>
+      </c>
+      <c r="J34" s="99"/>
+      <c r="K34" s="99"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="100" t="s">
         <v>96</v>
       </c>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="113" t="s">
+      <c r="N34" s="100"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="N34" s="113"/>
-      <c r="O34" s="113"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="114" t="s">
-        <v>98</v>
-      </c>
-      <c r="R34" s="114"/>
-      <c r="S34" s="114"/>
+      <c r="R34" s="101"/>
+      <c r="S34" s="101"/>
       <c r="T34" s="34"/>
-      <c r="U34" s="95" t="s">
-        <v>122</v>
-      </c>
-      <c r="V34" s="96"/>
-      <c r="W34" s="96"/>
-      <c r="X34" s="96"/>
-      <c r="Y34" s="96"/>
-      <c r="Z34" s="96"/>
-      <c r="AA34" s="96"/>
-      <c r="AB34" s="96"/>
-      <c r="AC34" s="96"/>
-      <c r="AD34" s="96"/>
-      <c r="AE34" s="96"/>
-      <c r="AF34" s="96"/>
+      <c r="U34" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="V34" s="63"/>
+      <c r="W34" s="63"/>
+      <c r="X34" s="63"/>
+      <c r="Y34" s="63"/>
+      <c r="Z34" s="63"/>
+      <c r="AA34" s="63"/>
+      <c r="AB34" s="63"/>
+      <c r="AC34" s="63"/>
+      <c r="AD34" s="63"/>
+      <c r="AE34" s="63"/>
+      <c r="AF34" s="63"/>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
@@ -2828,34 +2828,34 @@
       <c r="F35" s="36"/>
       <c r="G35" s="36"/>
       <c r="H35" s="42"/>
-      <c r="I35" s="95" t="s">
-        <v>99</v>
-      </c>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="97"/>
-      <c r="U35" s="95" t="s">
-        <v>123</v>
-      </c>
-      <c r="V35" s="96"/>
-      <c r="W35" s="96"/>
-      <c r="X35" s="96"/>
-      <c r="Y35" s="96"/>
-      <c r="Z35" s="96"/>
-      <c r="AA35" s="96"/>
-      <c r="AB35" s="96"/>
-      <c r="AC35" s="96"/>
-      <c r="AD35" s="96"/>
-      <c r="AE35" s="96"/>
-      <c r="AF35" s="96"/>
+      <c r="I35" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="63"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="63"/>
+      <c r="P35" s="63"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="63"/>
+      <c r="S35" s="63"/>
+      <c r="T35" s="77"/>
+      <c r="U35" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="V35" s="63"/>
+      <c r="W35" s="63"/>
+      <c r="X35" s="63"/>
+      <c r="Y35" s="63"/>
+      <c r="Z35" s="63"/>
+      <c r="AA35" s="63"/>
+      <c r="AB35" s="63"/>
+      <c r="AC35" s="63"/>
+      <c r="AD35" s="63"/>
+      <c r="AE35" s="63"/>
+      <c r="AF35" s="63"/>
     </row>
     <row r="36" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
@@ -2870,39 +2870,39 @@
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
       <c r="H36" s="42"/>
-      <c r="I36" s="109" t="s">
+      <c r="I36" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="J36" s="110"/>
-      <c r="K36" s="110"/>
+      <c r="J36" s="102"/>
+      <c r="K36" s="102"/>
       <c r="L36" s="35"/>
-      <c r="M36" s="89" t="s">
+      <c r="M36" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
       <c r="P36" s="35"/>
-      <c r="Q36" s="89" t="s">
+      <c r="Q36" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="R36" s="89"/>
-      <c r="S36" s="89"/>
+      <c r="R36" s="65"/>
+      <c r="S36" s="65"/>
       <c r="T36" s="34"/>
-      <c r="U36" s="88" t="s">
-        <v>124</v>
-      </c>
-      <c r="V36" s="89"/>
-      <c r="W36" s="89"/>
-      <c r="X36" s="89"/>
-      <c r="Y36" s="89"/>
+      <c r="U36" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="V36" s="65"/>
+      <c r="W36" s="65"/>
+      <c r="X36" s="65"/>
+      <c r="Y36" s="65"/>
       <c r="Z36" s="35"/>
-      <c r="AA36" s="89" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB36" s="89"/>
-      <c r="AC36" s="89"/>
-      <c r="AD36" s="89"/>
-      <c r="AE36" s="89"/>
+      <c r="AA36" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB36" s="65"/>
+      <c r="AC36" s="65"/>
+      <c r="AD36" s="65"/>
+      <c r="AE36" s="65"/>
       <c r="AF36" s="35"/>
     </row>
     <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2913,9 +2913,9 @@
       <c r="C37" s="36"/>
       <c r="D37" s="36"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="81"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="68"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -2928,32 +2928,32 @@
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="15"/>
-      <c r="U37" s="127" t="s">
-        <v>125</v>
-      </c>
-      <c r="V37" s="128"/>
-      <c r="W37" s="128"/>
-      <c r="X37" s="128"/>
-      <c r="Y37" s="128"/>
-      <c r="Z37" s="128"/>
-      <c r="AA37" s="128"/>
-      <c r="AB37" s="128"/>
-      <c r="AC37" s="128"/>
-      <c r="AD37" s="128"/>
-      <c r="AE37" s="128"/>
+      <c r="U37" s="78" t="s">
+        <v>124</v>
+      </c>
+      <c r="V37" s="79"/>
+      <c r="W37" s="79"/>
+      <c r="X37" s="79"/>
+      <c r="Y37" s="79"/>
+      <c r="Z37" s="79"/>
+      <c r="AA37" s="79"/>
+      <c r="AB37" s="79"/>
+      <c r="AC37" s="79"/>
+      <c r="AD37" s="79"/>
+      <c r="AE37" s="79"/>
       <c r="AF37" s="35"/>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="131"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="74"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
@@ -2966,17 +2966,17 @@
       <c r="R38" s="16"/>
       <c r="S38" s="16"/>
       <c r="T38" s="23"/>
-      <c r="U38" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="V38" s="72"/>
-      <c r="W38" s="72"/>
-      <c r="X38" s="72"/>
-      <c r="Y38" s="72"/>
-      <c r="Z38" s="72"/>
-      <c r="AA38" s="72"/>
-      <c r="AB38" s="72"/>
-      <c r="AC38" s="72"/>
+      <c r="U38" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="V38" s="67"/>
+      <c r="W38" s="67"/>
+      <c r="X38" s="67"/>
+      <c r="Y38" s="67"/>
+      <c r="Z38" s="67"/>
+      <c r="AA38" s="67"/>
+      <c r="AB38" s="67"/>
+      <c r="AC38" s="67"/>
       <c r="AD38" s="13"/>
       <c r="AE38" s="13"/>
       <c r="AF38" s="13"/>
@@ -3008,19 +3008,19 @@
       <c r="R39" s="16"/>
       <c r="S39" s="16"/>
       <c r="T39" s="23"/>
-      <c r="U39" s="127" t="s">
-        <v>127</v>
-      </c>
-      <c r="V39" s="128"/>
-      <c r="W39" s="128"/>
-      <c r="X39" s="128"/>
-      <c r="Y39" s="128"/>
-      <c r="Z39" s="128"/>
-      <c r="AA39" s="128"/>
-      <c r="AB39" s="128"/>
-      <c r="AC39" s="128"/>
-      <c r="AD39" s="128"/>
-      <c r="AE39" s="128"/>
+      <c r="U39" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="V39" s="79"/>
+      <c r="W39" s="79"/>
+      <c r="X39" s="79"/>
+      <c r="Y39" s="79"/>
+      <c r="Z39" s="79"/>
+      <c r="AA39" s="79"/>
+      <c r="AB39" s="79"/>
+      <c r="AC39" s="79"/>
+      <c r="AD39" s="79"/>
+      <c r="AE39" s="79"/>
       <c r="AF39" s="35"/>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
@@ -3050,58 +3050,58 @@
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
       <c r="T40" s="17"/>
-      <c r="U40" s="129" t="s">
-        <v>128</v>
-      </c>
-      <c r="V40" s="130"/>
-      <c r="W40" s="130"/>
-      <c r="X40" s="130"/>
-      <c r="Y40" s="130"/>
-      <c r="Z40" s="130"/>
-      <c r="AA40" s="130"/>
-      <c r="AB40" s="130"/>
-      <c r="AC40" s="130"/>
-      <c r="AD40" s="130"/>
-      <c r="AE40" s="130"/>
-      <c r="AF40" s="130"/>
+      <c r="U40" s="93" t="s">
+        <v>127</v>
+      </c>
+      <c r="V40" s="94"/>
+      <c r="W40" s="94"/>
+      <c r="X40" s="94"/>
+      <c r="Y40" s="94"/>
+      <c r="Z40" s="94"/>
+      <c r="AA40" s="94"/>
+      <c r="AB40" s="94"/>
+      <c r="AC40" s="94"/>
+      <c r="AD40" s="94"/>
+      <c r="AE40" s="94"/>
+      <c r="AF40" s="94"/>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A41" s="82" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="81"/>
-      <c r="I41" s="95" t="s">
-        <v>100</v>
-      </c>
-      <c r="J41" s="96"/>
-      <c r="K41" s="96"/>
-      <c r="L41" s="96"/>
-      <c r="M41" s="96"/>
-      <c r="N41" s="96"/>
-      <c r="O41" s="96"/>
-      <c r="P41" s="96"/>
-      <c r="Q41" s="96"/>
-      <c r="R41" s="96"/>
-      <c r="S41" s="96"/>
-      <c r="T41" s="97"/>
-      <c r="U41" s="129"/>
-      <c r="V41" s="130"/>
-      <c r="W41" s="130"/>
-      <c r="X41" s="130"/>
-      <c r="Y41" s="130"/>
-      <c r="Z41" s="130"/>
-      <c r="AA41" s="130"/>
-      <c r="AB41" s="130"/>
-      <c r="AC41" s="130"/>
-      <c r="AD41" s="130"/>
-      <c r="AE41" s="130"/>
-      <c r="AF41" s="130"/>
+      <c r="A41" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="68"/>
+      <c r="I41" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="63"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="63"/>
+      <c r="R41" s="63"/>
+      <c r="S41" s="63"/>
+      <c r="T41" s="77"/>
+      <c r="U41" s="93"/>
+      <c r="V41" s="94"/>
+      <c r="W41" s="94"/>
+      <c r="X41" s="94"/>
+      <c r="Y41" s="94"/>
+      <c r="Z41" s="94"/>
+      <c r="AA41" s="94"/>
+      <c r="AB41" s="94"/>
+      <c r="AC41" s="94"/>
+      <c r="AD41" s="94"/>
+      <c r="AE41" s="94"/>
+      <c r="AF41" s="94"/>
     </row>
     <row r="42" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
@@ -3115,33 +3115,33 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="95" t="s">
-        <v>101</v>
-      </c>
-      <c r="J42" s="96"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
-      <c r="M42" s="96"/>
-      <c r="N42" s="96"/>
-      <c r="O42" s="96"/>
-      <c r="P42" s="96"/>
-      <c r="Q42" s="96"/>
-      <c r="R42" s="96"/>
-      <c r="S42" s="96"/>
-      <c r="T42" s="97"/>
-      <c r="U42" s="127" t="s">
-        <v>129</v>
-      </c>
-      <c r="V42" s="128"/>
-      <c r="W42" s="128"/>
-      <c r="X42" s="128"/>
-      <c r="Y42" s="128"/>
-      <c r="Z42" s="128"/>
-      <c r="AA42" s="128"/>
-      <c r="AB42" s="128"/>
-      <c r="AC42" s="128"/>
-      <c r="AD42" s="128"/>
-      <c r="AE42" s="128"/>
+      <c r="I42" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="J42" s="63"/>
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="78" t="s">
+        <v>128</v>
+      </c>
+      <c r="V42" s="79"/>
+      <c r="W42" s="79"/>
+      <c r="X42" s="79"/>
+      <c r="Y42" s="79"/>
+      <c r="Z42" s="79"/>
+      <c r="AA42" s="79"/>
+      <c r="AB42" s="79"/>
+      <c r="AC42" s="79"/>
+      <c r="AD42" s="79"/>
+      <c r="AE42" s="79"/>
       <c r="AF42" s="35"/>
     </row>
     <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -3156,21 +3156,21 @@
       <c r="F43" s="43"/>
       <c r="G43" s="43"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="88" t="s">
-        <v>102</v>
-      </c>
-      <c r="J43" s="89"/>
-      <c r="K43" s="89"/>
-      <c r="L43" s="89"/>
-      <c r="M43" s="89"/>
+      <c r="I43" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="J43" s="65"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="89" t="s">
+      <c r="O43" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="P43" s="89"/>
-      <c r="Q43" s="89"/>
-      <c r="R43" s="89"/>
-      <c r="S43" s="89"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
+      <c r="R43" s="65"/>
+      <c r="S43" s="65"/>
       <c r="T43" s="34"/>
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
@@ -3197,61 +3197,61 @@
       <c r="F44" s="43"/>
       <c r="G44" s="43"/>
       <c r="H44" s="28"/>
-      <c r="I44" s="95" t="s">
-        <v>104</v>
-      </c>
-      <c r="J44" s="96"/>
-      <c r="K44" s="96"/>
-      <c r="L44" s="96"/>
-      <c r="M44" s="96"/>
-      <c r="N44" s="96"/>
-      <c r="O44" s="96"/>
-      <c r="P44" s="96"/>
-      <c r="Q44" s="96"/>
-      <c r="R44" s="96"/>
-      <c r="S44" s="96"/>
-      <c r="T44" s="97"/>
-      <c r="U44" s="132" t="s">
-        <v>130</v>
-      </c>
-      <c r="V44" s="133"/>
-      <c r="W44" s="133"/>
-      <c r="X44" s="133"/>
-      <c r="Y44" s="133"/>
-      <c r="Z44" s="133"/>
-      <c r="AA44" s="133"/>
-      <c r="AB44" s="133"/>
-      <c r="AC44" s="133"/>
-      <c r="AD44" s="133"/>
-      <c r="AE44" s="133"/>
-      <c r="AF44" s="133"/>
+      <c r="I44" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="63"/>
+      <c r="S44" s="63"/>
+      <c r="T44" s="77"/>
+      <c r="U44" s="75" t="s">
+        <v>129</v>
+      </c>
+      <c r="V44" s="76"/>
+      <c r="W44" s="76"/>
+      <c r="X44" s="76"/>
+      <c r="Y44" s="76"/>
+      <c r="Z44" s="76"/>
+      <c r="AA44" s="76"/>
+      <c r="AB44" s="76"/>
+      <c r="AC44" s="76"/>
+      <c r="AD44" s="76"/>
+      <c r="AE44" s="76"/>
+      <c r="AF44" s="76"/>
     </row>
     <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="71"/>
-      <c r="C45" s="71"/>
+      <c r="A45" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="69"/>
+      <c r="C45" s="69"/>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
       <c r="F45" s="48"/>
       <c r="G45" s="46"/>
       <c r="H45" s="47"/>
-      <c r="I45" s="88" t="s">
-        <v>43</v>
-      </c>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
-      <c r="M45" s="89"/>
+      <c r="I45" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="J45" s="65"/>
+      <c r="K45" s="65"/>
+      <c r="L45" s="65"/>
+      <c r="M45" s="65"/>
       <c r="N45" s="35"/>
-      <c r="O45" s="89" t="s">
+      <c r="O45" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="89"/>
-      <c r="Q45" s="89"/>
-      <c r="R45" s="89"/>
-      <c r="S45" s="89"/>
+      <c r="P45" s="65"/>
+      <c r="Q45" s="65"/>
+      <c r="R45" s="65"/>
+      <c r="S45" s="65"/>
       <c r="T45" s="34"/>
       <c r="U45" s="58"/>
       <c r="V45" s="59"/>
@@ -3267,30 +3267,30 @@
       <c r="AF45" s="59"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A46" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="90"/>
-      <c r="C46" s="90"/>
+      <c r="A46" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="70"/>
+      <c r="C46" s="70"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
       <c r="G46" s="39"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="95" t="s">
-        <v>105</v>
-      </c>
-      <c r="J46" s="96"/>
-      <c r="K46" s="96"/>
-      <c r="L46" s="96"/>
-      <c r="M46" s="96"/>
-      <c r="N46" s="96"/>
-      <c r="O46" s="96"/>
-      <c r="P46" s="96"/>
-      <c r="Q46" s="96"/>
-      <c r="R46" s="96"/>
-      <c r="S46" s="96"/>
-      <c r="T46" s="97"/>
+      <c r="I46" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="63"/>
+      <c r="P46" s="63"/>
+      <c r="Q46" s="63"/>
+      <c r="R46" s="63"/>
+      <c r="S46" s="63"/>
+      <c r="T46" s="77"/>
       <c r="U46" s="58"/>
       <c r="V46" s="59"/>
       <c r="W46" s="59"/>
@@ -3305,31 +3305,31 @@
       <c r="AF46" s="59"/>
     </row>
     <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="82" t="s">
-        <v>75</v>
-      </c>
-      <c r="B47" s="72"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="81"/>
-      <c r="I47" s="88" t="s">
-        <v>102</v>
-      </c>
-      <c r="J47" s="89"/>
-      <c r="K47" s="89"/>
-      <c r="L47" s="89"/>
-      <c r="M47" s="89"/>
+      <c r="A47" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="67"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="J47" s="65"/>
+      <c r="K47" s="65"/>
+      <c r="L47" s="65"/>
+      <c r="M47" s="65"/>
       <c r="N47" s="35"/>
-      <c r="O47" s="89" t="s">
+      <c r="O47" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="P47" s="89"/>
-      <c r="Q47" s="89"/>
-      <c r="R47" s="89"/>
-      <c r="S47" s="89"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="65"/>
+      <c r="R47" s="65"/>
+      <c r="S47" s="65"/>
       <c r="T47" s="34"/>
       <c r="U47" s="58"/>
       <c r="V47" s="59"/>
@@ -3346,31 +3346,31 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="73"/>
       <c r="C48" s="73"/>
       <c r="D48" s="73"/>
       <c r="E48" s="51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F48" s="49"/>
       <c r="G48" s="49"/>
       <c r="H48" s="11"/>
-      <c r="I48" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="J48" s="96"/>
-      <c r="K48" s="96"/>
-      <c r="L48" s="96"/>
-      <c r="M48" s="96"/>
-      <c r="N48" s="96"/>
-      <c r="O48" s="96"/>
-      <c r="P48" s="96"/>
-      <c r="Q48" s="96"/>
-      <c r="R48" s="96"/>
-      <c r="S48" s="96"/>
-      <c r="T48" s="97"/>
+      <c r="I48" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="63"/>
+      <c r="P48" s="63"/>
+      <c r="Q48" s="63"/>
+      <c r="R48" s="63"/>
+      <c r="S48" s="63"/>
+      <c r="T48" s="77"/>
       <c r="U48" s="58"/>
       <c r="V48" s="59"/>
       <c r="W48" s="59"/>
@@ -3385,31 +3385,31 @@
       <c r="AF48" s="59"/>
     </row>
     <row r="49" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="71" t="s">
+      <c r="A49" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="72"/>
-      <c r="C49" s="72"/>
+      <c r="B49" s="67"/>
+      <c r="C49" s="67"/>
       <c r="D49" s="44"/>
       <c r="E49" s="49"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="80"/>
-      <c r="I49" s="88" t="s">
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="119"/>
+      <c r="I49" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="J49" s="65"/>
+      <c r="K49" s="65"/>
+      <c r="L49" s="65"/>
+      <c r="M49" s="65"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="J49" s="89"/>
-      <c r="K49" s="89"/>
-      <c r="L49" s="89"/>
-      <c r="M49" s="89"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="P49" s="89"/>
-      <c r="Q49" s="89"/>
-      <c r="R49" s="89"/>
-      <c r="S49" s="89"/>
+      <c r="P49" s="65"/>
+      <c r="Q49" s="65"/>
+      <c r="R49" s="65"/>
+      <c r="S49" s="65"/>
       <c r="T49" s="34"/>
       <c r="U49" s="58"/>
       <c r="V49" s="59"/>
@@ -3425,16 +3425,16 @@
       <c r="AF49" s="59"/>
     </row>
     <row r="50" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B50" s="72"/>
-      <c r="C50" s="72"/>
+      <c r="A50" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
       <c r="D50" s="44"/>
       <c r="E50" s="49"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="77"/>
+      <c r="F50" s="131"/>
+      <c r="G50" s="131"/>
+      <c r="H50" s="132"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -3461,11 +3461,11 @@
       <c r="AF50" s="59"/>
     </row>
     <row r="51" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
+      <c r="A51" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="67"/>
+      <c r="C51" s="67"/>
       <c r="D51" s="44"/>
       <c r="E51" s="49"/>
       <c r="F51" s="50"/>
@@ -3498,14 +3498,14 @@
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A52" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
+        <v>79</v>
+      </c>
+      <c r="B52" s="67"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
       <c r="H52" s="11"/>
       <c r="I52" s="16"/>
       <c r="J52" s="16"/>
@@ -3521,16 +3521,16 @@
       <c r="T52" s="23"/>
     </row>
     <row r="53" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="72"/>
+      <c r="A53" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" s="67"/>
+      <c r="C53" s="67"/>
       <c r="D53" s="44"/>
       <c r="E53" s="49"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="72"/>
-      <c r="H53" s="80"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="119"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
@@ -3543,150 +3543,150 @@
       <c r="R53" s="13"/>
       <c r="S53" s="13"/>
       <c r="T53" s="2"/>
-      <c r="U53" s="125" t="s">
-        <v>131</v>
-      </c>
-      <c r="V53" s="126"/>
-      <c r="W53" s="126"/>
-      <c r="X53" s="126"/>
-      <c r="Y53" s="126"/>
-      <c r="Z53" s="126"/>
-      <c r="AA53" s="126"/>
-      <c r="AB53" s="126"/>
-      <c r="AC53" s="126"/>
-      <c r="AD53" s="126"/>
-      <c r="AE53" s="126"/>
-      <c r="AF53" s="126"/>
+      <c r="U53" s="91" t="s">
+        <v>130</v>
+      </c>
+      <c r="V53" s="92"/>
+      <c r="W53" s="92"/>
+      <c r="X53" s="92"/>
+      <c r="Y53" s="92"/>
+      <c r="Z53" s="92"/>
+      <c r="AA53" s="92"/>
+      <c r="AB53" s="92"/>
+      <c r="AC53" s="92"/>
+      <c r="AD53" s="92"/>
+      <c r="AE53" s="92"/>
+      <c r="AF53" s="92"/>
     </row>
     <row r="54" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B54" s="72"/>
-      <c r="C54" s="72"/>
+      <c r="A54" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="67"/>
+      <c r="C54" s="67"/>
       <c r="D54" s="44"/>
       <c r="E54" s="49"/>
-      <c r="F54" s="76"/>
-      <c r="G54" s="76"/>
-      <c r="H54" s="77"/>
-      <c r="I54" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="J54" s="96"/>
-      <c r="K54" s="96"/>
-      <c r="L54" s="96"/>
-      <c r="M54" s="96"/>
-      <c r="N54" s="96"/>
-      <c r="O54" s="96"/>
-      <c r="P54" s="96"/>
-      <c r="Q54" s="96"/>
-      <c r="R54" s="96"/>
-      <c r="S54" s="96"/>
-      <c r="T54" s="97"/>
-      <c r="U54" s="124" t="s">
-        <v>132</v>
-      </c>
-      <c r="V54" s="119"/>
-      <c r="W54" s="119"/>
-      <c r="X54" s="119"/>
-      <c r="Y54" s="119"/>
-      <c r="Z54" s="119"/>
-      <c r="AA54" s="119"/>
-      <c r="AB54" s="119"/>
-      <c r="AC54" s="119"/>
-      <c r="AD54" s="119"/>
-      <c r="AE54" s="119"/>
-      <c r="AF54" s="119"/>
+      <c r="F54" s="131"/>
+      <c r="G54" s="131"/>
+      <c r="H54" s="132"/>
+      <c r="I54" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="63"/>
+      <c r="M54" s="63"/>
+      <c r="N54" s="63"/>
+      <c r="O54" s="63"/>
+      <c r="P54" s="63"/>
+      <c r="Q54" s="63"/>
+      <c r="R54" s="63"/>
+      <c r="S54" s="63"/>
+      <c r="T54" s="77"/>
+      <c r="U54" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="V54" s="85"/>
+      <c r="W54" s="85"/>
+      <c r="X54" s="85"/>
+      <c r="Y54" s="85"/>
+      <c r="Z54" s="85"/>
+      <c r="AA54" s="85"/>
+      <c r="AB54" s="85"/>
+      <c r="AC54" s="85"/>
+      <c r="AD54" s="85"/>
+      <c r="AE54" s="85"/>
+      <c r="AF54" s="85"/>
     </row>
     <row r="55" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="72"/>
-      <c r="C55" s="72"/>
+      <c r="A55" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="67"/>
+      <c r="C55" s="67"/>
       <c r="D55" s="44"/>
       <c r="E55" s="49"/>
       <c r="F55" s="50"/>
       <c r="G55" s="50"/>
       <c r="H55" s="23"/>
-      <c r="I55" s="95" t="s">
-        <v>107</v>
-      </c>
-      <c r="J55" s="96"/>
-      <c r="K55" s="96"/>
-      <c r="L55" s="96"/>
-      <c r="M55" s="96"/>
-      <c r="N55" s="96"/>
-      <c r="O55" s="96"/>
-      <c r="P55" s="96"/>
-      <c r="Q55" s="96"/>
-      <c r="R55" s="96"/>
-      <c r="S55" s="96"/>
-      <c r="T55" s="97"/>
-      <c r="U55" s="124"/>
-      <c r="V55" s="119"/>
-      <c r="W55" s="119"/>
-      <c r="X55" s="119"/>
-      <c r="Y55" s="119"/>
-      <c r="Z55" s="119"/>
-      <c r="AA55" s="119"/>
-      <c r="AB55" s="119"/>
-      <c r="AC55" s="119"/>
-      <c r="AD55" s="119"/>
-      <c r="AE55" s="119"/>
-      <c r="AF55" s="119"/>
+      <c r="I55" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="63"/>
+      <c r="M55" s="63"/>
+      <c r="N55" s="63"/>
+      <c r="O55" s="63"/>
+      <c r="P55" s="63"/>
+      <c r="Q55" s="63"/>
+      <c r="R55" s="63"/>
+      <c r="S55" s="63"/>
+      <c r="T55" s="77"/>
+      <c r="U55" s="90"/>
+      <c r="V55" s="85"/>
+      <c r="W55" s="85"/>
+      <c r="X55" s="85"/>
+      <c r="Y55" s="85"/>
+      <c r="Z55" s="85"/>
+      <c r="AA55" s="85"/>
+      <c r="AB55" s="85"/>
+      <c r="AC55" s="85"/>
+      <c r="AD55" s="85"/>
+      <c r="AE55" s="85"/>
+      <c r="AF55" s="85"/>
     </row>
     <row r="56" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="72"/>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
+        <v>80</v>
+      </c>
+      <c r="B56" s="67"/>
+      <c r="C56" s="67"/>
+      <c r="D56" s="67"/>
+      <c r="E56" s="67"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="67"/>
       <c r="H56" s="11"/>
-      <c r="I56" s="88" t="s">
+      <c r="I56" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="J56" s="89"/>
-      <c r="K56" s="89"/>
+      <c r="J56" s="65"/>
+      <c r="K56" s="65"/>
       <c r="L56" s="33"/>
-      <c r="M56" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="N56" s="89"/>
-      <c r="O56" s="89"/>
-      <c r="P56" s="89"/>
-      <c r="Q56" s="89"/>
+      <c r="M56" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="N56" s="65"/>
+      <c r="O56" s="65"/>
+      <c r="P56" s="65"/>
+      <c r="Q56" s="65"/>
       <c r="R56" s="55"/>
       <c r="S56" s="55"/>
       <c r="T56" s="57"/>
-      <c r="U56" s="124"/>
-      <c r="V56" s="119"/>
-      <c r="W56" s="119"/>
-      <c r="X56" s="119"/>
-      <c r="Y56" s="119"/>
-      <c r="Z56" s="119"/>
-      <c r="AA56" s="119"/>
-      <c r="AB56" s="119"/>
-      <c r="AC56" s="119"/>
-      <c r="AD56" s="119"/>
-      <c r="AE56" s="119"/>
-      <c r="AF56" s="119"/>
+      <c r="U56" s="90"/>
+      <c r="V56" s="85"/>
+      <c r="W56" s="85"/>
+      <c r="X56" s="85"/>
+      <c r="Y56" s="85"/>
+      <c r="Z56" s="85"/>
+      <c r="AA56" s="85"/>
+      <c r="AB56" s="85"/>
+      <c r="AC56" s="85"/>
+      <c r="AD56" s="85"/>
+      <c r="AE56" s="85"/>
+      <c r="AF56" s="85"/>
     </row>
     <row r="57" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B57" s="72"/>
-      <c r="C57" s="72"/>
+      <c r="A57" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="67"/>
+      <c r="C57" s="67"/>
       <c r="D57" s="44"/>
       <c r="E57" s="49"/>
-      <c r="F57" s="72"/>
-      <c r="G57" s="72"/>
-      <c r="H57" s="80"/>
+      <c r="F57" s="67"/>
+      <c r="G57" s="67"/>
+      <c r="H57" s="119"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
@@ -3695,105 +3695,105 @@
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
-      <c r="Q57" s="107" t="s">
-        <v>109</v>
-      </c>
-      <c r="R57" s="107"/>
-      <c r="S57" s="107"/>
-      <c r="T57" s="108"/>
-      <c r="U57" s="124"/>
-      <c r="V57" s="119"/>
-      <c r="W57" s="119"/>
-      <c r="X57" s="119"/>
-      <c r="Y57" s="119"/>
-      <c r="Z57" s="119"/>
-      <c r="AA57" s="119"/>
-      <c r="AB57" s="119"/>
-      <c r="AC57" s="119"/>
-      <c r="AD57" s="119"/>
-      <c r="AE57" s="119"/>
-      <c r="AF57" s="119"/>
+      <c r="Q57" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="R57" s="71"/>
+      <c r="S57" s="71"/>
+      <c r="T57" s="72"/>
+      <c r="U57" s="90"/>
+      <c r="V57" s="85"/>
+      <c r="W57" s="85"/>
+      <c r="X57" s="85"/>
+      <c r="Y57" s="85"/>
+      <c r="Z57" s="85"/>
+      <c r="AA57" s="85"/>
+      <c r="AB57" s="85"/>
+      <c r="AC57" s="85"/>
+      <c r="AD57" s="85"/>
+      <c r="AE57" s="85"/>
+      <c r="AF57" s="85"/>
     </row>
     <row r="58" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B58" s="72"/>
-      <c r="C58" s="72"/>
+      <c r="A58" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="67"/>
+      <c r="C58" s="67"/>
       <c r="D58" s="44"/>
       <c r="E58" s="49"/>
-      <c r="F58" s="76"/>
-      <c r="G58" s="76"/>
-      <c r="H58" s="77"/>
-      <c r="I58" s="95" t="s">
-        <v>111</v>
-      </c>
-      <c r="J58" s="96"/>
-      <c r="K58" s="96"/>
-      <c r="L58" s="96"/>
-      <c r="M58" s="96"/>
-      <c r="N58" s="96"/>
-      <c r="O58" s="96"/>
-      <c r="P58" s="96"/>
-      <c r="Q58" s="96"/>
-      <c r="R58" s="96"/>
-      <c r="S58" s="96"/>
-      <c r="T58" s="97"/>
+      <c r="F58" s="131"/>
+      <c r="G58" s="131"/>
+      <c r="H58" s="132"/>
+      <c r="I58" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
+      <c r="L58" s="63"/>
+      <c r="M58" s="63"/>
+      <c r="N58" s="63"/>
+      <c r="O58" s="63"/>
+      <c r="P58" s="63"/>
+      <c r="Q58" s="63"/>
+      <c r="R58" s="63"/>
+      <c r="S58" s="63"/>
+      <c r="T58" s="77"/>
       <c r="U58" s="1"/>
       <c r="AF58" s="13"/>
     </row>
     <row r="59" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B59" s="72"/>
-      <c r="C59" s="72"/>
+      <c r="A59" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="67"/>
+      <c r="C59" s="67"/>
       <c r="D59" s="44"/>
       <c r="E59" s="49"/>
       <c r="F59" s="50"/>
       <c r="G59" s="50"/>
       <c r="H59" s="23"/>
-      <c r="I59" s="109" t="s">
-        <v>110</v>
-      </c>
-      <c r="J59" s="98"/>
-      <c r="K59" s="98"/>
+      <c r="I59" s="96" t="s">
+        <v>109</v>
+      </c>
+      <c r="J59" s="97"/>
+      <c r="K59" s="97"/>
       <c r="L59" s="33"/>
-      <c r="M59" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="N59" s="89"/>
-      <c r="O59" s="89"/>
-      <c r="P59" s="89"/>
-      <c r="Q59" s="89"/>
+      <c r="M59" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="N59" s="65"/>
+      <c r="O59" s="65"/>
+      <c r="P59" s="65"/>
+      <c r="Q59" s="65"/>
       <c r="R59" s="55"/>
       <c r="S59" s="55"/>
       <c r="T59" s="57"/>
       <c r="U59" s="1"/>
-      <c r="V59" s="115" t="s">
-        <v>133</v>
-      </c>
-      <c r="W59" s="116"/>
-      <c r="X59" s="116"/>
-      <c r="Y59" s="116"/>
-      <c r="Z59" s="116"/>
-      <c r="AA59" s="116"/>
-      <c r="AB59" s="116"/>
-      <c r="AC59" s="116"/>
-      <c r="AD59" s="116"/>
-      <c r="AE59" s="117"/>
+      <c r="V59" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="W59" s="82"/>
+      <c r="X59" s="82"/>
+      <c r="Y59" s="82"/>
+      <c r="Z59" s="82"/>
+      <c r="AA59" s="82"/>
+      <c r="AB59" s="82"/>
+      <c r="AC59" s="82"/>
+      <c r="AD59" s="82"/>
+      <c r="AE59" s="83"/>
       <c r="AF59" s="13"/>
     </row>
     <row r="60" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="73" t="s">
-        <v>82</v>
-      </c>
-      <c r="B60" s="72"/>
-      <c r="C60" s="72"/>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="72"/>
+        <v>81</v>
+      </c>
+      <c r="B60" s="67"/>
+      <c r="C60" s="67"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="67"/>
+      <c r="F60" s="67"/>
+      <c r="G60" s="67"/>
       <c r="H60" s="11"/>
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
@@ -3803,171 +3803,171 @@
       <c r="N60" s="13"/>
       <c r="O60" s="13"/>
       <c r="P60" s="13"/>
-      <c r="Q60" s="107" t="s">
-        <v>109</v>
-      </c>
-      <c r="R60" s="107"/>
-      <c r="S60" s="107"/>
-      <c r="T60" s="108"/>
+      <c r="Q60" s="71" t="s">
+        <v>108</v>
+      </c>
+      <c r="R60" s="71"/>
+      <c r="S60" s="71"/>
+      <c r="T60" s="72"/>
       <c r="U60" s="1"/>
-      <c r="V60" s="118"/>
-      <c r="W60" s="119"/>
-      <c r="X60" s="119"/>
-      <c r="Y60" s="119"/>
-      <c r="Z60" s="119"/>
-      <c r="AA60" s="119"/>
-      <c r="AB60" s="119"/>
-      <c r="AC60" s="119"/>
-      <c r="AD60" s="119"/>
-      <c r="AE60" s="120"/>
+      <c r="V60" s="84"/>
+      <c r="W60" s="85"/>
+      <c r="X60" s="85"/>
+      <c r="Y60" s="85"/>
+      <c r="Z60" s="85"/>
+      <c r="AA60" s="85"/>
+      <c r="AB60" s="85"/>
+      <c r="AC60" s="85"/>
+      <c r="AD60" s="85"/>
+      <c r="AE60" s="86"/>
       <c r="AF60" s="13"/>
     </row>
     <row r="61" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" s="72"/>
-      <c r="C61" s="72"/>
+      <c r="A61" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="67"/>
+      <c r="C61" s="67"/>
       <c r="D61" s="44"/>
       <c r="E61" s="49"/>
-      <c r="F61" s="72"/>
-      <c r="G61" s="72"/>
-      <c r="H61" s="80"/>
-      <c r="I61" s="95" t="s">
+      <c r="F61" s="67"/>
+      <c r="G61" s="67"/>
+      <c r="H61" s="119"/>
+      <c r="I61" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="J61" s="96"/>
-      <c r="K61" s="96"/>
-      <c r="L61" s="96"/>
-      <c r="M61" s="96"/>
-      <c r="N61" s="96"/>
-      <c r="O61" s="96"/>
-      <c r="P61" s="96"/>
-      <c r="Q61" s="96"/>
-      <c r="R61" s="96"/>
-      <c r="S61" s="96"/>
-      <c r="T61" s="97"/>
+      <c r="J61" s="63"/>
+      <c r="K61" s="63"/>
+      <c r="L61" s="63"/>
+      <c r="M61" s="63"/>
+      <c r="N61" s="63"/>
+      <c r="O61" s="63"/>
+      <c r="P61" s="63"/>
+      <c r="Q61" s="63"/>
+      <c r="R61" s="63"/>
+      <c r="S61" s="63"/>
+      <c r="T61" s="77"/>
       <c r="U61" s="1"/>
-      <c r="V61" s="118"/>
-      <c r="W61" s="119"/>
-      <c r="X61" s="119"/>
-      <c r="Y61" s="119"/>
-      <c r="Z61" s="119"/>
-      <c r="AA61" s="119"/>
-      <c r="AB61" s="119"/>
-      <c r="AC61" s="119"/>
-      <c r="AD61" s="119"/>
-      <c r="AE61" s="120"/>
+      <c r="V61" s="84"/>
+      <c r="W61" s="85"/>
+      <c r="X61" s="85"/>
+      <c r="Y61" s="85"/>
+      <c r="Z61" s="85"/>
+      <c r="AA61" s="85"/>
+      <c r="AB61" s="85"/>
+      <c r="AC61" s="85"/>
+      <c r="AD61" s="85"/>
+      <c r="AE61" s="86"/>
       <c r="AF61" s="13"/>
     </row>
     <row r="62" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B62" s="72"/>
-      <c r="C62" s="72"/>
+      <c r="A62" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="67"/>
+      <c r="C62" s="67"/>
       <c r="D62" s="44"/>
       <c r="E62" s="49"/>
-      <c r="F62" s="76"/>
-      <c r="G62" s="76"/>
-      <c r="H62" s="77"/>
-      <c r="I62" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="J62" s="106"/>
-      <c r="K62" s="106"/>
+      <c r="F62" s="131"/>
+      <c r="G62" s="131"/>
+      <c r="H62" s="132"/>
+      <c r="I62" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="J62" s="95"/>
+      <c r="K62" s="95"/>
       <c r="L62" s="33"/>
-      <c r="M62" s="89" t="s">
+      <c r="M62" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="N62" s="89"/>
-      <c r="O62" s="89"/>
+      <c r="N62" s="65"/>
+      <c r="O62" s="65"/>
       <c r="P62" s="33"/>
-      <c r="Q62" s="89" t="s">
+      <c r="Q62" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="R62" s="89"/>
-      <c r="S62" s="89"/>
+      <c r="R62" s="65"/>
+      <c r="S62" s="65"/>
       <c r="T62" s="34"/>
       <c r="U62" s="1"/>
-      <c r="V62" s="118"/>
-      <c r="W62" s="119"/>
-      <c r="X62" s="119"/>
-      <c r="Y62" s="119"/>
-      <c r="Z62" s="119"/>
-      <c r="AA62" s="119"/>
-      <c r="AB62" s="119"/>
-      <c r="AC62" s="119"/>
-      <c r="AD62" s="119"/>
-      <c r="AE62" s="120"/>
+      <c r="V62" s="84"/>
+      <c r="W62" s="85"/>
+      <c r="X62" s="85"/>
+      <c r="Y62" s="85"/>
+      <c r="Z62" s="85"/>
+      <c r="AA62" s="85"/>
+      <c r="AB62" s="85"/>
+      <c r="AC62" s="85"/>
+      <c r="AD62" s="85"/>
+      <c r="AE62" s="86"/>
       <c r="AF62" s="13"/>
     </row>
     <row r="63" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B63" s="72"/>
-      <c r="C63" s="72"/>
+      <c r="A63" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B63" s="67"/>
+      <c r="C63" s="67"/>
       <c r="D63" s="44"/>
       <c r="E63" s="49"/>
       <c r="F63" s="50"/>
       <c r="G63" s="50"/>
       <c r="H63" s="23"/>
-      <c r="I63" s="95" t="s">
+      <c r="I63" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="J63" s="96"/>
-      <c r="K63" s="96"/>
-      <c r="L63" s="96"/>
-      <c r="M63" s="96"/>
-      <c r="N63" s="96"/>
-      <c r="O63" s="96"/>
-      <c r="P63" s="96"/>
-      <c r="Q63" s="96"/>
-      <c r="R63" s="96"/>
-      <c r="S63" s="96"/>
-      <c r="T63" s="97"/>
+      <c r="J63" s="63"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="63"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="63"/>
+      <c r="O63" s="63"/>
+      <c r="P63" s="63"/>
+      <c r="Q63" s="63"/>
+      <c r="R63" s="63"/>
+      <c r="S63" s="63"/>
+      <c r="T63" s="77"/>
       <c r="U63" s="1"/>
-      <c r="V63" s="121"/>
-      <c r="W63" s="122"/>
-      <c r="X63" s="122"/>
-      <c r="Y63" s="122"/>
-      <c r="Z63" s="122"/>
-      <c r="AA63" s="122"/>
-      <c r="AB63" s="122"/>
-      <c r="AC63" s="122"/>
-      <c r="AD63" s="122"/>
-      <c r="AE63" s="123"/>
+      <c r="V63" s="87"/>
+      <c r="W63" s="88"/>
+      <c r="X63" s="88"/>
+      <c r="Y63" s="88"/>
+      <c r="Z63" s="88"/>
+      <c r="AA63" s="88"/>
+      <c r="AB63" s="88"/>
+      <c r="AC63" s="88"/>
+      <c r="AD63" s="88"/>
+      <c r="AE63" s="89"/>
       <c r="AF63" s="13"/>
     </row>
     <row r="64" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="73" t="s">
-        <v>83</v>
-      </c>
-      <c r="B64" s="72"/>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="72"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
+        <v>82</v>
+      </c>
+      <c r="B64" s="67"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="67"/>
+      <c r="G64" s="67"/>
       <c r="H64" s="11"/>
-      <c r="I64" s="88" t="s">
-        <v>112</v>
-      </c>
-      <c r="J64" s="106"/>
-      <c r="K64" s="106"/>
+      <c r="I64" s="64" t="s">
+        <v>111</v>
+      </c>
+      <c r="J64" s="95"/>
+      <c r="K64" s="95"/>
       <c r="L64" s="33"/>
-      <c r="M64" s="89" t="s">
+      <c r="M64" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="N64" s="89"/>
-      <c r="O64" s="89"/>
+      <c r="N64" s="65"/>
+      <c r="O64" s="65"/>
       <c r="P64" s="33"/>
-      <c r="Q64" s="89" t="s">
+      <c r="Q64" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="R64" s="89"/>
-      <c r="S64" s="89"/>
+      <c r="R64" s="65"/>
+      <c r="S64" s="65"/>
       <c r="T64" s="34"/>
       <c r="U64" s="1"/>
       <c r="V64" s="20"/>
@@ -3981,16 +3981,16 @@
       <c r="AD64" s="1"/>
     </row>
     <row r="65" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="72"/>
+      <c r="A65" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="67"/>
+      <c r="C65" s="67"/>
       <c r="D65" s="45"/>
       <c r="E65" s="52"/>
-      <c r="F65" s="74"/>
-      <c r="G65" s="74"/>
-      <c r="H65" s="75"/>
+      <c r="F65" s="129"/>
+      <c r="G65" s="129"/>
+      <c r="H65" s="130"/>
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
@@ -4004,30 +4004,30 @@
       <c r="S65" s="13"/>
       <c r="T65" s="2"/>
       <c r="U65" s="1"/>
-      <c r="V65" s="62" t="s">
-        <v>134</v>
-      </c>
-      <c r="W65" s="63"/>
-      <c r="X65" s="63"/>
-      <c r="Y65" s="63"/>
-      <c r="Z65" s="63"/>
-      <c r="AA65" s="63"/>
-      <c r="AB65" s="63"/>
-      <c r="AC65" s="63"/>
-      <c r="AD65" s="63"/>
-      <c r="AE65" s="64"/>
+      <c r="V65" s="120" t="s">
+        <v>133</v>
+      </c>
+      <c r="W65" s="121"/>
+      <c r="X65" s="121"/>
+      <c r="Y65" s="121"/>
+      <c r="Z65" s="121"/>
+      <c r="AA65" s="121"/>
+      <c r="AB65" s="121"/>
+      <c r="AC65" s="121"/>
+      <c r="AD65" s="121"/>
+      <c r="AE65" s="122"/>
     </row>
     <row r="66" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="72"/>
-      <c r="C66" s="72"/>
+      <c r="A66" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" s="67"/>
+      <c r="C66" s="67"/>
       <c r="D66" s="45"/>
       <c r="E66" s="52"/>
-      <c r="F66" s="78"/>
-      <c r="G66" s="78"/>
-      <c r="H66" s="79"/>
+      <c r="F66" s="133"/>
+      <c r="G66" s="133"/>
+      <c r="H66" s="134"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
       <c r="K66" s="13"/>
@@ -4041,23 +4041,23 @@
       <c r="S66" s="13"/>
       <c r="T66" s="26"/>
       <c r="U66" s="1"/>
-      <c r="V66" s="65"/>
-      <c r="W66" s="66"/>
-      <c r="X66" s="66"/>
-      <c r="Y66" s="66"/>
-      <c r="Z66" s="66"/>
-      <c r="AA66" s="66"/>
-      <c r="AB66" s="66"/>
-      <c r="AC66" s="66"/>
-      <c r="AD66" s="66"/>
-      <c r="AE66" s="67"/>
+      <c r="V66" s="123"/>
+      <c r="W66" s="124"/>
+      <c r="X66" s="124"/>
+      <c r="Y66" s="124"/>
+      <c r="Z66" s="124"/>
+      <c r="AA66" s="124"/>
+      <c r="AB66" s="124"/>
+      <c r="AC66" s="124"/>
+      <c r="AD66" s="124"/>
+      <c r="AE66" s="125"/>
     </row>
     <row r="67" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="72"/>
-      <c r="C67" s="72"/>
+      <c r="A67" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="67"/>
+      <c r="C67" s="67"/>
       <c r="D67" s="45"/>
       <c r="E67" s="52"/>
       <c r="F67" s="53"/>
@@ -4076,16 +4076,16 @@
       <c r="S67" s="13"/>
       <c r="T67" s="2"/>
       <c r="U67" s="1"/>
-      <c r="V67" s="68"/>
-      <c r="W67" s="69"/>
-      <c r="X67" s="69"/>
-      <c r="Y67" s="69"/>
-      <c r="Z67" s="69"/>
-      <c r="AA67" s="69"/>
-      <c r="AB67" s="69"/>
-      <c r="AC67" s="69"/>
-      <c r="AD67" s="69"/>
-      <c r="AE67" s="70"/>
+      <c r="V67" s="126"/>
+      <c r="W67" s="127"/>
+      <c r="X67" s="127"/>
+      <c r="Y67" s="127"/>
+      <c r="Z67" s="127"/>
+      <c r="AA67" s="127"/>
+      <c r="AB67" s="127"/>
+      <c r="AC67" s="127"/>
+      <c r="AD67" s="127"/>
+      <c r="AE67" s="128"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
@@ -4124,6 +4124,148 @@
     </row>
   </sheetData>
   <mergeCells count="166">
+    <mergeCell ref="V65:AE67"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="I54:T54"/>
+    <mergeCell ref="I55:T55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="M56:Q56"/>
+    <mergeCell ref="I61:T61"/>
+    <mergeCell ref="I63:T63"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="F49:H49"/>
+    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="U22:W22"/>
+    <mergeCell ref="Y22:AC22"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="I23:T23"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="H1:Z3"/>
+    <mergeCell ref="I20:T20"/>
+    <mergeCell ref="I21:T21"/>
+    <mergeCell ref="U20:AF20"/>
+    <mergeCell ref="U21:W21"/>
+    <mergeCell ref="Y21:AA21"/>
+    <mergeCell ref="AC21:AE21"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B1:G3"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="U31:W31"/>
+    <mergeCell ref="U34:AF34"/>
+    <mergeCell ref="U35:AF35"/>
+    <mergeCell ref="O30:S30"/>
+    <mergeCell ref="I25:T25"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="I27:T27"/>
+    <mergeCell ref="I28:M28"/>
+    <mergeCell ref="O28:S28"/>
+    <mergeCell ref="I29:T29"/>
+    <mergeCell ref="AC27:AF27"/>
+    <mergeCell ref="U28:AF28"/>
+    <mergeCell ref="U30:AF30"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="AD29:AE29"/>
+    <mergeCell ref="I35:T35"/>
+    <mergeCell ref="I64:K64"/>
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="Q57:T57"/>
+    <mergeCell ref="I58:T58"/>
+    <mergeCell ref="Q60:T60"/>
+    <mergeCell ref="M59:Q59"/>
+    <mergeCell ref="I59:K59"/>
+    <mergeCell ref="AC31:AE31"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="V59:AE63"/>
+    <mergeCell ref="U54:AF57"/>
+    <mergeCell ref="U53:AF53"/>
+    <mergeCell ref="U39:AE39"/>
+    <mergeCell ref="U40:AF41"/>
+    <mergeCell ref="U42:AE42"/>
+    <mergeCell ref="I49:M49"/>
+    <mergeCell ref="O43:S43"/>
+    <mergeCell ref="O45:S45"/>
+    <mergeCell ref="O47:S47"/>
+    <mergeCell ref="O49:S49"/>
+    <mergeCell ref="I44:T44"/>
+    <mergeCell ref="I46:T46"/>
+    <mergeCell ref="I48:T48"/>
+    <mergeCell ref="I41:T41"/>
+    <mergeCell ref="I31:T31"/>
+    <mergeCell ref="I32:M32"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="I33:T33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q34:S34"/>
     <mergeCell ref="U24:AF24"/>
     <mergeCell ref="I30:M30"/>
     <mergeCell ref="A41:H41"/>
@@ -4148,148 +4290,6 @@
     <mergeCell ref="AA36:AE36"/>
     <mergeCell ref="U38:AC38"/>
     <mergeCell ref="U37:AE37"/>
-    <mergeCell ref="AC31:AE31"/>
-    <mergeCell ref="Y31:AA31"/>
-    <mergeCell ref="V59:AE63"/>
-    <mergeCell ref="U54:AF57"/>
-    <mergeCell ref="U53:AF53"/>
-    <mergeCell ref="U39:AE39"/>
-    <mergeCell ref="U40:AF41"/>
-    <mergeCell ref="U42:AE42"/>
-    <mergeCell ref="I49:M49"/>
-    <mergeCell ref="O43:S43"/>
-    <mergeCell ref="O45:S45"/>
-    <mergeCell ref="O47:S47"/>
-    <mergeCell ref="O49:S49"/>
-    <mergeCell ref="I44:T44"/>
-    <mergeCell ref="I46:T46"/>
-    <mergeCell ref="I48:T48"/>
-    <mergeCell ref="I64:K64"/>
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="Q57:T57"/>
-    <mergeCell ref="I58:T58"/>
-    <mergeCell ref="Q60:T60"/>
-    <mergeCell ref="M59:Q59"/>
-    <mergeCell ref="I59:K59"/>
-    <mergeCell ref="I41:T41"/>
-    <mergeCell ref="I31:T31"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="I33:T33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="I28:M28"/>
-    <mergeCell ref="O28:S28"/>
-    <mergeCell ref="I29:T29"/>
-    <mergeCell ref="AC27:AF27"/>
-    <mergeCell ref="U28:AF28"/>
-    <mergeCell ref="U30:AF30"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="AD29:AE29"/>
-    <mergeCell ref="I35:T35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="Q36:S36"/>
-    <mergeCell ref="U31:W31"/>
-    <mergeCell ref="U34:AF34"/>
-    <mergeCell ref="U35:AF35"/>
-    <mergeCell ref="O30:S30"/>
-    <mergeCell ref="I25:T25"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="Q26:S26"/>
-    <mergeCell ref="I27:T27"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="Q22:S22"/>
-    <mergeCell ref="I23:T23"/>
-    <mergeCell ref="I24:M24"/>
-    <mergeCell ref="O24:S24"/>
-    <mergeCell ref="H1:Z3"/>
-    <mergeCell ref="I20:T20"/>
-    <mergeCell ref="I21:T21"/>
-    <mergeCell ref="U20:AF20"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="Y21:AA21"/>
-    <mergeCell ref="AC21:AE21"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B1:G3"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="Y22:AC22"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A30:H30"/>
-    <mergeCell ref="F49:H49"/>
-    <mergeCell ref="A66:C66"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F57:H57"/>
-    <mergeCell ref="V65:AE67"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="F58:H58"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="I54:T54"/>
-    <mergeCell ref="I55:T55"/>
-    <mergeCell ref="I56:K56"/>
-    <mergeCell ref="M56:Q56"/>
-    <mergeCell ref="I61:T61"/>
-    <mergeCell ref="I63:T63"/>
-    <mergeCell ref="I62:K62"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: add options in order form generating file
</commit_message>
<xml_diff>
--- a/server/orders/OrderFormTmpEng.xlsx
+++ b/server/orders/OrderFormTmpEng.xlsx
@@ -723,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -843,145 +843,136 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -989,6 +980,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1089,59 +1083,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="56882"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2762250" y="609600"/>
-          <a:ext cx="2028825" cy="2562225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
@@ -1163,7 +1104,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1207,7 +1148,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1222,49 +1163,6 @@
         <a:xfrm flipH="1">
           <a:off x="2017186" y="11596650"/>
           <a:ext cx="163742" cy="471526"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>56553</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>180646</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Рисунок 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="43233" t="72110"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4895850" y="2371724"/>
-          <a:ext cx="2714028" cy="733097"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1294,7 +1192,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1313,59 +1211,6 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="43117" b="36431"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4952999" y="657225"/>
-          <a:ext cx="2676525" cy="1628775"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1391,7 +1236,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1435,7 +1280,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1479,7 +1324,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1494,6 +1339,50 @@
         <a:xfrm>
           <a:off x="1704975" y="11087100"/>
           <a:ext cx="702656" cy="271126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762250" y="647700"/>
+          <a:ext cx="4743450" cy="2562225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1797,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:C62"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1810,35 +1699,35 @@
   <sheetData>
     <row r="1" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7"/>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="105" t="s">
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="103"/>
+      <c r="U1" s="103"/>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
       <c r="AA1" s="8"/>
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
@@ -1848,31 +1737,31 @@
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
-      <c r="X2" s="105"/>
-      <c r="Y2" s="105"/>
-      <c r="Z2" s="105"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
       <c r="AC2" s="8"/>
@@ -1882,31 +1771,31 @@
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
-      <c r="N3" s="105"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="105"/>
-      <c r="Q3" s="105"/>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
-      <c r="U3" s="105"/>
-      <c r="V3" s="105"/>
-      <c r="W3" s="105"/>
-      <c r="X3" s="105"/>
-      <c r="Y3" s="105"/>
-      <c r="Z3" s="105"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="103"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
+      <c r="X3" s="103"/>
+      <c r="Y3" s="103"/>
+      <c r="Z3" s="103"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
@@ -1915,70 +1804,70 @@
       <c r="AF3" s="8"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="68"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="59"/>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="59"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A6" s="107" t="s">
+      <c r="A6" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="68"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="109"/>
-      <c r="C7" s="109"/>
-      <c r="D7" s="109"/>
-      <c r="E7" s="109"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="109"/>
-      <c r="H7" s="110"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="107"/>
+      <c r="D7" s="107"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="108"/>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="68"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -1987,10 +1876,10 @@
       <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="67"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="36"/>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
@@ -1999,10 +1888,10 @@
       <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="67"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
@@ -2011,10 +1900,10 @@
       <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="67"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
@@ -2023,10 +1912,10 @@
       <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="112"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
@@ -2035,65 +1924,65 @@
       <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
       <c r="H14" s="37"/>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="111"/>
-      <c r="D15" s="111"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
       <c r="E15" s="38"/>
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
       <c r="H15" s="40"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="59"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="36"/>
       <c r="G17" s="36"/>
       <c r="H17" s="41"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A18" s="113" t="s">
+      <c r="A18" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="113"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="36"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
       <c r="H18" s="2"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -2121,17 +2010,17 @@
       <c r="AF18" s="10"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="113"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="36"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="2"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
@@ -2159,166 +2048,166 @@
       <c r="AF19" s="13"/>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="111" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="113"/>
+      <c r="B20" s="111"/>
       <c r="C20" s="36"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="69" t="s">
+      <c r="E20" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="62" t="s">
+      <c r="I20" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="J20" s="63"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="63"/>
-      <c r="M20" s="63"/>
-      <c r="N20" s="63"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="63"/>
-      <c r="S20" s="63"/>
-      <c r="T20" s="77"/>
-      <c r="U20" s="62" t="s">
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="V20" s="63"/>
-      <c r="W20" s="63"/>
-      <c r="X20" s="63"/>
-      <c r="Y20" s="63"/>
-      <c r="Z20" s="63"/>
-      <c r="AA20" s="63"/>
-      <c r="AB20" s="63"/>
-      <c r="AC20" s="63"/>
-      <c r="AD20" s="63"/>
-      <c r="AE20" s="63"/>
-      <c r="AF20" s="63"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
+      <c r="Y20" s="67"/>
+      <c r="Z20" s="67"/>
+      <c r="AA20" s="67"/>
+      <c r="AB20" s="67"/>
+      <c r="AC20" s="67"/>
+      <c r="AD20" s="67"/>
+      <c r="AE20" s="67"/>
+      <c r="AF20" s="67"/>
     </row>
     <row r="21" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="113" t="s">
+      <c r="A21" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="113"/>
+      <c r="B21" s="111"/>
       <c r="C21" s="36"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="69" t="s">
+      <c r="E21" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="62" t="s">
+      <c r="I21" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="63"/>
-      <c r="Q21" s="63"/>
-      <c r="R21" s="63"/>
-      <c r="S21" s="63"/>
-      <c r="T21" s="77"/>
-      <c r="U21" s="64" t="s">
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="68"/>
+      <c r="U21" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="V21" s="65"/>
-      <c r="W21" s="65"/>
+      <c r="V21" s="70"/>
+      <c r="W21" s="70"/>
       <c r="X21" s="35"/>
-      <c r="Y21" s="65" t="s">
+      <c r="Y21" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="Z21" s="65"/>
-      <c r="AA21" s="65"/>
+      <c r="Z21" s="70"/>
+      <c r="AA21" s="70"/>
       <c r="AB21" s="35"/>
-      <c r="AC21" s="97" t="s">
+      <c r="AC21" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="AD21" s="97"/>
-      <c r="AE21" s="97"/>
+      <c r="AD21" s="77"/>
+      <c r="AE21" s="77"/>
       <c r="AF21" s="35"/>
     </row>
     <row r="22" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="113" t="s">
+      <c r="A22" s="111" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="113"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="36"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="64" t="s">
+      <c r="I22" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
       <c r="L22" s="35"/>
-      <c r="M22" s="65" t="s">
+      <c r="M22" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="N22" s="65"/>
-      <c r="O22" s="65"/>
+      <c r="N22" s="70"/>
+      <c r="O22" s="70"/>
       <c r="P22" s="35"/>
-      <c r="Q22" s="65" t="s">
+      <c r="Q22" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="R22" s="65"/>
-      <c r="S22" s="65"/>
+      <c r="R22" s="70"/>
+      <c r="S22" s="70"/>
       <c r="T22" s="34"/>
-      <c r="U22" s="64" t="s">
+      <c r="U22" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="V22" s="65"/>
-      <c r="W22" s="65"/>
+      <c r="V22" s="70"/>
+      <c r="W22" s="70"/>
       <c r="X22" s="35"/>
-      <c r="Y22" s="65" t="s">
+      <c r="Y22" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="Z22" s="65"/>
-      <c r="AA22" s="65"/>
-      <c r="AB22" s="65"/>
-      <c r="AC22" s="65"/>
-      <c r="AD22" s="56"/>
-      <c r="AE22" s="56"/>
-      <c r="AF22" s="56"/>
+      <c r="Z22" s="70"/>
+      <c r="AA22" s="70"/>
+      <c r="AB22" s="70"/>
+      <c r="AC22" s="70"/>
+      <c r="AD22" s="77"/>
+      <c r="AE22" s="77"/>
+      <c r="AF22" s="77"/>
     </row>
     <row r="23" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="66"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="114"/>
-      <c r="I23" s="62" t="s">
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="77"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="67"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+      <c r="T23" s="68"/>
       <c r="U23" s="13"/>
       <c r="V23" s="13"/>
       <c r="W23" s="13"/>
@@ -2327,12 +2216,12 @@
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
       <c r="AB23" s="13"/>
-      <c r="AC23" s="71" t="s">
+      <c r="AC23" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="AD23" s="71"/>
-      <c r="AE23" s="71"/>
-      <c r="AF23" s="72"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
+      <c r="AF23" s="61"/>
       <c r="AG23" s="19"/>
     </row>
     <row r="24" spans="1:33" ht="15" x14ac:dyDescent="0.2">
@@ -2340,160 +2229,160 @@
         <v>64</v>
       </c>
       <c r="B24" s="29"/>
-      <c r="C24" s="115" t="s">
+      <c r="C24" s="113" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="116"/>
+      <c r="D24" s="114"/>
       <c r="E24" s="29"/>
-      <c r="F24" s="115" t="s">
+      <c r="F24" s="113" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="115"/>
+      <c r="G24" s="113"/>
       <c r="H24" s="30"/>
-      <c r="I24" s="64" t="s">
+      <c r="I24" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="95"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="95"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
       <c r="N24" s="35"/>
-      <c r="O24" s="65" t="s">
+      <c r="O24" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="65"/>
+      <c r="P24" s="70"/>
+      <c r="Q24" s="70"/>
+      <c r="R24" s="70"/>
+      <c r="S24" s="70"/>
       <c r="T24" s="54"/>
-      <c r="U24" s="62" t="s">
+      <c r="U24" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="V24" s="63"/>
-      <c r="W24" s="63"/>
-      <c r="X24" s="63"/>
-      <c r="Y24" s="63"/>
-      <c r="Z24" s="63"/>
-      <c r="AA24" s="63"/>
-      <c r="AB24" s="63"/>
-      <c r="AC24" s="63"/>
-      <c r="AD24" s="63"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
+      <c r="V24" s="67"/>
+      <c r="W24" s="67"/>
+      <c r="X24" s="67"/>
+      <c r="Y24" s="67"/>
+      <c r="Z24" s="67"/>
+      <c r="AA24" s="67"/>
+      <c r="AB24" s="67"/>
+      <c r="AC24" s="67"/>
+      <c r="AD24" s="67"/>
+      <c r="AE24" s="67"/>
+      <c r="AF24" s="67"/>
     </row>
     <row r="25" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
       <c r="E25" s="36"/>
       <c r="F25" s="36"/>
       <c r="G25" s="36"/>
       <c r="H25" s="42"/>
-      <c r="I25" s="62" t="s">
+      <c r="I25" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
-      <c r="L25" s="63"/>
-      <c r="M25" s="63"/>
-      <c r="N25" s="63"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="63"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="63"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="77"/>
-      <c r="U25" s="64" t="s">
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
+      <c r="Q25" s="67"/>
+      <c r="R25" s="67"/>
+      <c r="S25" s="67"/>
+      <c r="T25" s="68"/>
+      <c r="U25" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="V25" s="65"/>
-      <c r="W25" s="65"/>
+      <c r="V25" s="70"/>
+      <c r="W25" s="70"/>
       <c r="X25" s="35"/>
-      <c r="Y25" s="65" t="s">
+      <c r="Y25" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="Z25" s="65"/>
-      <c r="AA25" s="65"/>
+      <c r="Z25" s="70"/>
+      <c r="AA25" s="70"/>
       <c r="AB25" s="35"/>
-      <c r="AC25" s="65" t="s">
+      <c r="AC25" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AD25" s="65"/>
-      <c r="AE25" s="65"/>
+      <c r="AD25" s="70"/>
+      <c r="AE25" s="70"/>
       <c r="AF25" s="35"/>
     </row>
     <row r="26" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
       <c r="G26" s="36"/>
       <c r="H26" s="42"/>
-      <c r="I26" s="104" t="s">
+      <c r="I26" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="J26" s="80"/>
-      <c r="K26" s="80"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
       <c r="L26" s="35"/>
-      <c r="M26" s="95" t="s">
+      <c r="M26" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="N26" s="95"/>
-      <c r="O26" s="95"/>
+      <c r="N26" s="97"/>
+      <c r="O26" s="97"/>
       <c r="P26" s="35"/>
-      <c r="Q26" s="65" t="s">
+      <c r="Q26" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="R26" s="65"/>
-      <c r="S26" s="65"/>
+      <c r="R26" s="70"/>
+      <c r="S26" s="70"/>
       <c r="T26" s="34"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
       <c r="W26" s="13"/>
       <c r="X26" s="13"/>
-      <c r="Y26" s="65" t="s">
+      <c r="Y26" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="Z26" s="65"/>
-      <c r="AA26" s="65"/>
-      <c r="AB26" s="65"/>
-      <c r="AC26" s="65"/>
-      <c r="AD26" s="56"/>
-      <c r="AE26" s="56"/>
-      <c r="AF26" s="56"/>
+      <c r="Z26" s="70"/>
+      <c r="AA26" s="70"/>
+      <c r="AB26" s="70"/>
+      <c r="AC26" s="70"/>
+      <c r="AD26" s="77"/>
+      <c r="AE26" s="77"/>
+      <c r="AF26" s="77"/>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="66"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="62" t="s">
+      <c r="I27" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="77"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="67"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="67"/>
+      <c r="R27" s="67"/>
+      <c r="S27" s="67"/>
+      <c r="T27" s="68"/>
       <c r="U27" s="13"/>
       <c r="V27" s="13"/>
       <c r="W27" s="13"/>
@@ -2502,144 +2391,144 @@
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
       <c r="AB27" s="13"/>
-      <c r="AC27" s="71" t="s">
+      <c r="AC27" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="AD27" s="71"/>
-      <c r="AE27" s="71"/>
-      <c r="AF27" s="72"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="61"/>
     </row>
     <row r="28" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="31"/>
-      <c r="C28" s="117" t="s">
+      <c r="C28" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="D28" s="118"/>
+      <c r="D28" s="116"/>
       <c r="E28" s="31"/>
-      <c r="F28" s="117" t="s">
+      <c r="F28" s="115" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="117"/>
+      <c r="G28" s="115"/>
       <c r="H28" s="32"/>
-      <c r="I28" s="64" t="s">
+      <c r="I28" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="70"/>
       <c r="N28" s="35"/>
-      <c r="O28" s="65" t="s">
+      <c r="O28" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="65"/>
-      <c r="R28" s="65"/>
-      <c r="S28" s="65"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="70"/>
+      <c r="R28" s="70"/>
+      <c r="S28" s="70"/>
       <c r="T28" s="34"/>
-      <c r="U28" s="62" t="s">
+      <c r="U28" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="V28" s="63"/>
-      <c r="W28" s="63"/>
-      <c r="X28" s="63"/>
-      <c r="Y28" s="63"/>
-      <c r="Z28" s="63"/>
-      <c r="AA28" s="63"/>
-      <c r="AB28" s="63"/>
-      <c r="AC28" s="63"/>
-      <c r="AD28" s="63"/>
-      <c r="AE28" s="63"/>
-      <c r="AF28" s="63"/>
+      <c r="V28" s="67"/>
+      <c r="W28" s="67"/>
+      <c r="X28" s="67"/>
+      <c r="Y28" s="67"/>
+      <c r="Z28" s="67"/>
+      <c r="AA28" s="67"/>
+      <c r="AB28" s="67"/>
+      <c r="AC28" s="67"/>
+      <c r="AD28" s="67"/>
+      <c r="AE28" s="67"/>
+      <c r="AF28" s="67"/>
     </row>
     <row r="29" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="62" t="s">
+      <c r="B29" s="58"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="63"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="63"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="63"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="77"/>
-      <c r="U29" s="64" t="s">
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="67"/>
+      <c r="P29" s="67"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="67"/>
+      <c r="S29" s="67"/>
+      <c r="T29" s="68"/>
+      <c r="U29" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="V29" s="65"/>
-      <c r="W29" s="65"/>
+      <c r="V29" s="70"/>
+      <c r="W29" s="70"/>
       <c r="X29" s="35"/>
-      <c r="Y29" s="65" t="s">
+      <c r="Y29" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="Z29" s="65"/>
-      <c r="AA29" s="65"/>
-      <c r="AB29" s="65"/>
+      <c r="Z29" s="70"/>
+      <c r="AA29" s="70"/>
+      <c r="AB29" s="70"/>
       <c r="AC29" s="35"/>
-      <c r="AD29" s="65" t="s">
+      <c r="AD29" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="AE29" s="65"/>
+      <c r="AE29" s="70"/>
       <c r="AF29" s="35"/>
     </row>
     <row r="30" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="64" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="J30" s="65"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="65"/>
-      <c r="M30" s="65"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="70"/>
       <c r="N30" s="35"/>
-      <c r="O30" s="65" t="s">
+      <c r="O30" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="65"/>
-      <c r="R30" s="65"/>
-      <c r="S30" s="65"/>
+      <c r="P30" s="70"/>
+      <c r="Q30" s="70"/>
+      <c r="R30" s="70"/>
+      <c r="S30" s="70"/>
       <c r="T30" s="34"/>
-      <c r="U30" s="62" t="s">
+      <c r="U30" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="V30" s="63"/>
-      <c r="W30" s="63"/>
-      <c r="X30" s="63"/>
-      <c r="Y30" s="63"/>
-      <c r="Z30" s="63"/>
-      <c r="AA30" s="63"/>
-      <c r="AB30" s="63"/>
-      <c r="AC30" s="63"/>
-      <c r="AD30" s="63"/>
-      <c r="AE30" s="63"/>
-      <c r="AF30" s="63"/>
+      <c r="V30" s="67"/>
+      <c r="W30" s="67"/>
+      <c r="X30" s="67"/>
+      <c r="Y30" s="67"/>
+      <c r="Z30" s="67"/>
+      <c r="AA30" s="67"/>
+      <c r="AB30" s="67"/>
+      <c r="AC30" s="67"/>
+      <c r="AD30" s="67"/>
+      <c r="AE30" s="67"/>
+      <c r="AF30" s="67"/>
     </row>
     <row r="31" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
@@ -2654,37 +2543,37 @@
       <c r="F31" s="36"/>
       <c r="G31" s="36"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="62" t="s">
+      <c r="I31" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="J31" s="63"/>
-      <c r="K31" s="63"/>
-      <c r="L31" s="63"/>
-      <c r="M31" s="63"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="63"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="77"/>
-      <c r="U31" s="103" t="s">
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="68"/>
+      <c r="U31" s="100" t="s">
         <v>120</v>
       </c>
-      <c r="V31" s="100"/>
-      <c r="W31" s="100"/>
+      <c r="V31" s="80"/>
+      <c r="W31" s="80"/>
       <c r="X31" s="35"/>
-      <c r="Y31" s="80" t="s">
+      <c r="Y31" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="80"/>
-      <c r="AA31" s="80"/>
+      <c r="Z31" s="102"/>
+      <c r="AA31" s="102"/>
       <c r="AB31" s="35"/>
-      <c r="AC31" s="80" t="s">
+      <c r="AC31" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="AD31" s="80"/>
-      <c r="AE31" s="80"/>
+      <c r="AD31" s="102"/>
+      <c r="AE31" s="102"/>
       <c r="AF31" s="35"/>
     </row>
     <row r="32" spans="1:33" ht="15" x14ac:dyDescent="0.2">
@@ -2700,21 +2589,21 @@
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
       <c r="H32" s="42"/>
-      <c r="I32" s="64" t="s">
+      <c r="I32" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="J32" s="65"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="65"/>
-      <c r="M32" s="65"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="70"/>
       <c r="N32" s="35"/>
-      <c r="O32" s="65" t="s">
+      <c r="O32" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="P32" s="65"/>
-      <c r="Q32" s="65"/>
-      <c r="R32" s="65"/>
-      <c r="S32" s="65"/>
+      <c r="P32" s="70"/>
+      <c r="Q32" s="70"/>
+      <c r="R32" s="70"/>
+      <c r="S32" s="70"/>
       <c r="T32" s="34"/>
       <c r="U32" s="14"/>
       <c r="V32" s="14"/>
@@ -2742,20 +2631,20 @@
       <c r="F33" s="36"/>
       <c r="G33" s="36"/>
       <c r="H33" s="42"/>
-      <c r="I33" s="62" t="s">
+      <c r="I33" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="J33" s="63"/>
-      <c r="K33" s="63"/>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="77"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="67"/>
+      <c r="T33" s="68"/>
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
       <c r="W33" s="13"/>
@@ -2782,38 +2671,38 @@
       <c r="F34" s="36"/>
       <c r="G34" s="36"/>
       <c r="H34" s="42"/>
-      <c r="I34" s="98" t="s">
+      <c r="I34" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
       <c r="L34" s="35"/>
-      <c r="M34" s="100" t="s">
+      <c r="M34" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="N34" s="100"/>
-      <c r="O34" s="100"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
       <c r="P34" s="35"/>
-      <c r="Q34" s="101" t="s">
+      <c r="Q34" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="R34" s="101"/>
-      <c r="S34" s="101"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="81"/>
       <c r="T34" s="34"/>
-      <c r="U34" s="62" t="s">
+      <c r="U34" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="V34" s="63"/>
-      <c r="W34" s="63"/>
-      <c r="X34" s="63"/>
-      <c r="Y34" s="63"/>
-      <c r="Z34" s="63"/>
-      <c r="AA34" s="63"/>
-      <c r="AB34" s="63"/>
-      <c r="AC34" s="63"/>
-      <c r="AD34" s="63"/>
-      <c r="AE34" s="63"/>
-      <c r="AF34" s="63"/>
+      <c r="V34" s="67"/>
+      <c r="W34" s="67"/>
+      <c r="X34" s="67"/>
+      <c r="Y34" s="67"/>
+      <c r="Z34" s="67"/>
+      <c r="AA34" s="67"/>
+      <c r="AB34" s="67"/>
+      <c r="AC34" s="67"/>
+      <c r="AD34" s="67"/>
+      <c r="AE34" s="67"/>
+      <c r="AF34" s="67"/>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
@@ -2828,34 +2717,34 @@
       <c r="F35" s="36"/>
       <c r="G35" s="36"/>
       <c r="H35" s="42"/>
-      <c r="I35" s="62" t="s">
+      <c r="I35" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="J35" s="63"/>
-      <c r="K35" s="63"/>
-      <c r="L35" s="63"/>
-      <c r="M35" s="63"/>
-      <c r="N35" s="63"/>
-      <c r="O35" s="63"/>
-      <c r="P35" s="63"/>
-      <c r="Q35" s="63"/>
-      <c r="R35" s="63"/>
-      <c r="S35" s="63"/>
-      <c r="T35" s="77"/>
-      <c r="U35" s="62" t="s">
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="67"/>
+      <c r="M35" s="67"/>
+      <c r="N35" s="67"/>
+      <c r="O35" s="67"/>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="67"/>
+      <c r="S35" s="67"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="V35" s="63"/>
-      <c r="W35" s="63"/>
-      <c r="X35" s="63"/>
-      <c r="Y35" s="63"/>
-      <c r="Z35" s="63"/>
-      <c r="AA35" s="63"/>
-      <c r="AB35" s="63"/>
-      <c r="AC35" s="63"/>
-      <c r="AD35" s="63"/>
-      <c r="AE35" s="63"/>
-      <c r="AF35" s="63"/>
+      <c r="V35" s="67"/>
+      <c r="W35" s="67"/>
+      <c r="X35" s="67"/>
+      <c r="Y35" s="67"/>
+      <c r="Z35" s="67"/>
+      <c r="AA35" s="67"/>
+      <c r="AB35" s="67"/>
+      <c r="AC35" s="67"/>
+      <c r="AD35" s="67"/>
+      <c r="AE35" s="67"/>
+      <c r="AF35" s="67"/>
     </row>
     <row r="36" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
@@ -2870,39 +2759,39 @@
       <c r="F36" s="36"/>
       <c r="G36" s="36"/>
       <c r="H36" s="42"/>
-      <c r="I36" s="96" t="s">
+      <c r="I36" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="J36" s="102"/>
-      <c r="K36" s="102"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="99"/>
       <c r="L36" s="35"/>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="N36" s="65"/>
-      <c r="O36" s="65"/>
+      <c r="N36" s="70"/>
+      <c r="O36" s="70"/>
       <c r="P36" s="35"/>
-      <c r="Q36" s="65" t="s">
+      <c r="Q36" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="R36" s="65"/>
-      <c r="S36" s="65"/>
+      <c r="R36" s="70"/>
+      <c r="S36" s="70"/>
       <c r="T36" s="34"/>
-      <c r="U36" s="64" t="s">
+      <c r="U36" s="69" t="s">
         <v>123</v>
       </c>
-      <c r="V36" s="65"/>
-      <c r="W36" s="65"/>
-      <c r="X36" s="65"/>
-      <c r="Y36" s="65"/>
+      <c r="V36" s="70"/>
+      <c r="W36" s="70"/>
+      <c r="X36" s="70"/>
+      <c r="Y36" s="70"/>
       <c r="Z36" s="35"/>
-      <c r="AA36" s="65" t="s">
+      <c r="AA36" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="AB36" s="65"/>
-      <c r="AC36" s="65"/>
-      <c r="AD36" s="65"/>
-      <c r="AE36" s="65"/>
+      <c r="AB36" s="70"/>
+      <c r="AC36" s="70"/>
+      <c r="AD36" s="70"/>
+      <c r="AE36" s="70"/>
       <c r="AF36" s="35"/>
     </row>
     <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2913,9 +2802,9 @@
       <c r="C37" s="36"/>
       <c r="D37" s="36"/>
       <c r="E37" s="3"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="67"/>
-      <c r="H37" s="68"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="59"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -2928,32 +2817,32 @@
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="15"/>
-      <c r="U37" s="78" t="s">
+      <c r="U37" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="V37" s="79"/>
-      <c r="W37" s="79"/>
-      <c r="X37" s="79"/>
-      <c r="Y37" s="79"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-      <c r="AB37" s="79"/>
-      <c r="AC37" s="79"/>
-      <c r="AD37" s="79"/>
-      <c r="AE37" s="79"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="72"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="72"/>
+      <c r="AB37" s="72"/>
+      <c r="AC37" s="72"/>
+      <c r="AD37" s="72"/>
+      <c r="AE37" s="72"/>
       <c r="AF37" s="35"/>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="66"/>
-      <c r="D38" s="66"/>
-      <c r="E38" s="66"/>
-      <c r="F38" s="66"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="74"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="63"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
@@ -2966,17 +2855,17 @@
       <c r="R38" s="16"/>
       <c r="S38" s="16"/>
       <c r="T38" s="23"/>
-      <c r="U38" s="69" t="s">
+      <c r="U38" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="V38" s="67"/>
-      <c r="W38" s="67"/>
-      <c r="X38" s="67"/>
-      <c r="Y38" s="67"/>
-      <c r="Z38" s="67"/>
-      <c r="AA38" s="67"/>
-      <c r="AB38" s="67"/>
-      <c r="AC38" s="67"/>
+      <c r="V38" s="58"/>
+      <c r="W38" s="58"/>
+      <c r="X38" s="58"/>
+      <c r="Y38" s="58"/>
+      <c r="Z38" s="58"/>
+      <c r="AA38" s="58"/>
+      <c r="AB38" s="58"/>
+      <c r="AC38" s="58"/>
       <c r="AD38" s="13"/>
       <c r="AE38" s="13"/>
       <c r="AF38" s="13"/>
@@ -3008,19 +2897,19 @@
       <c r="R39" s="16"/>
       <c r="S39" s="16"/>
       <c r="T39" s="23"/>
-      <c r="U39" s="78" t="s">
+      <c r="U39" s="71" t="s">
         <v>126</v>
       </c>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-      <c r="AB39" s="79"/>
-      <c r="AC39" s="79"/>
-      <c r="AD39" s="79"/>
-      <c r="AE39" s="79"/>
+      <c r="V39" s="72"/>
+      <c r="W39" s="72"/>
+      <c r="X39" s="72"/>
+      <c r="Y39" s="72"/>
+      <c r="Z39" s="72"/>
+      <c r="AA39" s="72"/>
+      <c r="AB39" s="72"/>
+      <c r="AC39" s="72"/>
+      <c r="AD39" s="72"/>
+      <c r="AE39" s="72"/>
       <c r="AF39" s="35"/>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.2">
@@ -3050,58 +2939,58 @@
       <c r="R40" s="16"/>
       <c r="S40" s="16"/>
       <c r="T40" s="17"/>
-      <c r="U40" s="93" t="s">
+      <c r="U40" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="V40" s="94"/>
-      <c r="W40" s="94"/>
-      <c r="X40" s="94"/>
-      <c r="Y40" s="94"/>
-      <c r="Z40" s="94"/>
-      <c r="AA40" s="94"/>
-      <c r="AB40" s="94"/>
-      <c r="AC40" s="94"/>
-      <c r="AD40" s="94"/>
-      <c r="AE40" s="94"/>
-      <c r="AF40" s="94"/>
+      <c r="V40" s="95"/>
+      <c r="W40" s="95"/>
+      <c r="X40" s="95"/>
+      <c r="Y40" s="95"/>
+      <c r="Z40" s="95"/>
+      <c r="AA40" s="95"/>
+      <c r="AB40" s="95"/>
+      <c r="AC40" s="95"/>
+      <c r="AD40" s="95"/>
+      <c r="AE40" s="95"/>
+      <c r="AF40" s="95"/>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="67"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="62" t="s">
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="59"/>
+      <c r="I41" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="J41" s="63"/>
-      <c r="K41" s="63"/>
-      <c r="L41" s="63"/>
-      <c r="M41" s="63"/>
-      <c r="N41" s="63"/>
-      <c r="O41" s="63"/>
-      <c r="P41" s="63"/>
-      <c r="Q41" s="63"/>
-      <c r="R41" s="63"/>
-      <c r="S41" s="63"/>
-      <c r="T41" s="77"/>
-      <c r="U41" s="93"/>
-      <c r="V41" s="94"/>
-      <c r="W41" s="94"/>
-      <c r="X41" s="94"/>
-      <c r="Y41" s="94"/>
-      <c r="Z41" s="94"/>
-      <c r="AA41" s="94"/>
-      <c r="AB41" s="94"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
-      <c r="AF41" s="94"/>
+      <c r="J41" s="67"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="67"/>
+      <c r="N41" s="67"/>
+      <c r="O41" s="67"/>
+      <c r="P41" s="67"/>
+      <c r="Q41" s="67"/>
+      <c r="R41" s="67"/>
+      <c r="S41" s="67"/>
+      <c r="T41" s="68"/>
+      <c r="U41" s="94"/>
+      <c r="V41" s="95"/>
+      <c r="W41" s="95"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="95"/>
+      <c r="Z41" s="95"/>
+      <c r="AA41" s="95"/>
+      <c r="AB41" s="95"/>
+      <c r="AC41" s="95"/>
+      <c r="AD41" s="95"/>
+      <c r="AE41" s="95"/>
+      <c r="AF41" s="95"/>
     </row>
     <row r="42" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
@@ -3115,33 +3004,33 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
       <c r="H42" s="28"/>
-      <c r="I42" s="62" t="s">
+      <c r="I42" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="63"/>
-      <c r="Q42" s="63"/>
-      <c r="R42" s="63"/>
-      <c r="S42" s="63"/>
-      <c r="T42" s="77"/>
-      <c r="U42" s="78" t="s">
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="67"/>
+      <c r="Q42" s="67"/>
+      <c r="R42" s="67"/>
+      <c r="S42" s="67"/>
+      <c r="T42" s="68"/>
+      <c r="U42" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="V42" s="79"/>
-      <c r="W42" s="79"/>
-      <c r="X42" s="79"/>
-      <c r="Y42" s="79"/>
-      <c r="Z42" s="79"/>
-      <c r="AA42" s="79"/>
-      <c r="AB42" s="79"/>
-      <c r="AC42" s="79"/>
-      <c r="AD42" s="79"/>
-      <c r="AE42" s="79"/>
+      <c r="V42" s="72"/>
+      <c r="W42" s="72"/>
+      <c r="X42" s="72"/>
+      <c r="Y42" s="72"/>
+      <c r="Z42" s="72"/>
+      <c r="AA42" s="72"/>
+      <c r="AB42" s="72"/>
+      <c r="AC42" s="72"/>
+      <c r="AD42" s="72"/>
+      <c r="AE42" s="72"/>
       <c r="AF42" s="35"/>
     </row>
     <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -3156,21 +3045,21 @@
       <c r="F43" s="43"/>
       <c r="G43" s="43"/>
       <c r="H43" s="27"/>
-      <c r="I43" s="64" t="s">
+      <c r="I43" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="J43" s="65"/>
-      <c r="K43" s="65"/>
-      <c r="L43" s="65"/>
-      <c r="M43" s="65"/>
+      <c r="J43" s="70"/>
+      <c r="K43" s="70"/>
+      <c r="L43" s="70"/>
+      <c r="M43" s="70"/>
       <c r="N43" s="35"/>
-      <c r="O43" s="65" t="s">
+      <c r="O43" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="P43" s="65"/>
-      <c r="Q43" s="65"/>
-      <c r="R43" s="65"/>
-      <c r="S43" s="65"/>
+      <c r="P43" s="70"/>
+      <c r="Q43" s="70"/>
+      <c r="R43" s="70"/>
+      <c r="S43" s="70"/>
       <c r="T43" s="34"/>
       <c r="U43" s="14"/>
       <c r="V43" s="14"/>
@@ -3197,244 +3086,244 @@
       <c r="F44" s="43"/>
       <c r="G44" s="43"/>
       <c r="H44" s="28"/>
-      <c r="I44" s="62" t="s">
+      <c r="I44" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="J44" s="63"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="63"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="63"/>
-      <c r="P44" s="63"/>
-      <c r="Q44" s="63"/>
-      <c r="R44" s="63"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="77"/>
-      <c r="U44" s="75" t="s">
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
+      <c r="L44" s="67"/>
+      <c r="M44" s="67"/>
+      <c r="N44" s="67"/>
+      <c r="O44" s="67"/>
+      <c r="P44" s="67"/>
+      <c r="Q44" s="67"/>
+      <c r="R44" s="67"/>
+      <c r="S44" s="67"/>
+      <c r="T44" s="68"/>
+      <c r="U44" s="64" t="s">
         <v>129</v>
       </c>
-      <c r="V44" s="76"/>
-      <c r="W44" s="76"/>
-      <c r="X44" s="76"/>
-      <c r="Y44" s="76"/>
-      <c r="Z44" s="76"/>
-      <c r="AA44" s="76"/>
-      <c r="AB44" s="76"/>
-      <c r="AC44" s="76"/>
-      <c r="AD44" s="76"/>
-      <c r="AE44" s="76"/>
-      <c r="AF44" s="76"/>
+      <c r="V44" s="65"/>
+      <c r="W44" s="65"/>
+      <c r="X44" s="65"/>
+      <c r="Y44" s="65"/>
+      <c r="Z44" s="65"/>
+      <c r="AA44" s="65"/>
+      <c r="AB44" s="65"/>
+      <c r="AC44" s="65"/>
+      <c r="AD44" s="65"/>
+      <c r="AE44" s="65"/>
+      <c r="AF44" s="65"/>
     </row>
     <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="69" t="s">
+      <c r="A45" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B45" s="69"/>
-      <c r="C45" s="69"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
       <c r="F45" s="48"/>
       <c r="G45" s="46"/>
       <c r="H45" s="47"/>
-      <c r="I45" s="64" t="s">
+      <c r="I45" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="J45" s="65"/>
-      <c r="K45" s="65"/>
-      <c r="L45" s="65"/>
-      <c r="M45" s="65"/>
+      <c r="J45" s="70"/>
+      <c r="K45" s="70"/>
+      <c r="L45" s="70"/>
+      <c r="M45" s="70"/>
       <c r="N45" s="35"/>
-      <c r="O45" s="65" t="s">
+      <c r="O45" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="65"/>
-      <c r="Q45" s="65"/>
-      <c r="R45" s="65"/>
-      <c r="S45" s="65"/>
+      <c r="P45" s="70"/>
+      <c r="Q45" s="70"/>
+      <c r="R45" s="70"/>
+      <c r="S45" s="70"/>
       <c r="T45" s="34"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="59"/>
-      <c r="W45" s="59"/>
-      <c r="X45" s="59"/>
-      <c r="Y45" s="59"/>
-      <c r="Z45" s="59"/>
-      <c r="AA45" s="59"/>
-      <c r="AB45" s="59"/>
-      <c r="AC45" s="59"/>
-      <c r="AD45" s="59"/>
-      <c r="AE45" s="59"/>
-      <c r="AF45" s="59"/>
+      <c r="U45" s="73"/>
+      <c r="V45" s="74"/>
+      <c r="W45" s="74"/>
+      <c r="X45" s="74"/>
+      <c r="Y45" s="74"/>
+      <c r="Z45" s="74"/>
+      <c r="AA45" s="74"/>
+      <c r="AB45" s="74"/>
+      <c r="AC45" s="74"/>
+      <c r="AD45" s="74"/>
+      <c r="AE45" s="74"/>
+      <c r="AF45" s="74"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A46" s="70" t="s">
+      <c r="A46" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="70"/>
-      <c r="C46" s="70"/>
+      <c r="B46" s="56"/>
+      <c r="C46" s="56"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
       <c r="G46" s="39"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="62" t="s">
+      <c r="I46" s="66" t="s">
         <v>104</v>
       </c>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
-      <c r="L46" s="63"/>
-      <c r="M46" s="63"/>
-      <c r="N46" s="63"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="63"/>
-      <c r="Q46" s="63"/>
-      <c r="R46" s="63"/>
-      <c r="S46" s="63"/>
-      <c r="T46" s="77"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="59"/>
-      <c r="W46" s="59"/>
-      <c r="X46" s="59"/>
-      <c r="Y46" s="59"/>
-      <c r="Z46" s="59"/>
-      <c r="AA46" s="59"/>
-      <c r="AB46" s="59"/>
-      <c r="AC46" s="59"/>
-      <c r="AD46" s="59"/>
-      <c r="AE46" s="59"/>
-      <c r="AF46" s="59"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
+      <c r="L46" s="67"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
+      <c r="O46" s="67"/>
+      <c r="P46" s="67"/>
+      <c r="Q46" s="67"/>
+      <c r="R46" s="67"/>
+      <c r="S46" s="67"/>
+      <c r="T46" s="68"/>
+      <c r="U46" s="73"/>
+      <c r="V46" s="74"/>
+      <c r="W46" s="74"/>
+      <c r="X46" s="74"/>
+      <c r="Y46" s="74"/>
+      <c r="Z46" s="74"/>
+      <c r="AA46" s="74"/>
+      <c r="AB46" s="74"/>
+      <c r="AC46" s="74"/>
+      <c r="AD46" s="74"/>
+      <c r="AE46" s="74"/>
+      <c r="AF46" s="74"/>
     </row>
     <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="67"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="64" t="s">
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="J47" s="65"/>
-      <c r="K47" s="65"/>
-      <c r="L47" s="65"/>
-      <c r="M47" s="65"/>
+      <c r="J47" s="70"/>
+      <c r="K47" s="70"/>
+      <c r="L47" s="70"/>
+      <c r="M47" s="70"/>
       <c r="N47" s="35"/>
-      <c r="O47" s="65" t="s">
+      <c r="O47" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="P47" s="65"/>
-      <c r="Q47" s="65"/>
-      <c r="R47" s="65"/>
-      <c r="S47" s="65"/>
+      <c r="P47" s="70"/>
+      <c r="Q47" s="70"/>
+      <c r="R47" s="70"/>
+      <c r="S47" s="70"/>
       <c r="T47" s="34"/>
-      <c r="U47" s="58"/>
-      <c r="V47" s="59"/>
-      <c r="W47" s="59"/>
-      <c r="X47" s="59"/>
-      <c r="Y47" s="59"/>
-      <c r="Z47" s="59"/>
-      <c r="AA47" s="59"/>
-      <c r="AB47" s="59"/>
-      <c r="AC47" s="59"/>
-      <c r="AD47" s="59"/>
-      <c r="AE47" s="59"/>
-      <c r="AF47" s="59"/>
+      <c r="U47" s="73"/>
+      <c r="V47" s="74"/>
+      <c r="W47" s="74"/>
+      <c r="X47" s="74"/>
+      <c r="Y47" s="74"/>
+      <c r="Z47" s="74"/>
+      <c r="AA47" s="74"/>
+      <c r="AB47" s="74"/>
+      <c r="AC47" s="74"/>
+      <c r="AD47" s="74"/>
+      <c r="AE47" s="74"/>
+      <c r="AF47" s="74"/>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A48" s="73" t="s">
+      <c r="A48" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="73"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
       <c r="E48" s="51" t="s">
         <v>76</v>
       </c>
       <c r="F48" s="49"/>
       <c r="G48" s="49"/>
       <c r="H48" s="11"/>
-      <c r="I48" s="62" t="s">
+      <c r="I48" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="J48" s="63"/>
-      <c r="K48" s="63"/>
-      <c r="L48" s="63"/>
-      <c r="M48" s="63"/>
-      <c r="N48" s="63"/>
-      <c r="O48" s="63"/>
-      <c r="P48" s="63"/>
-      <c r="Q48" s="63"/>
-      <c r="R48" s="63"/>
-      <c r="S48" s="63"/>
-      <c r="T48" s="77"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="59"/>
-      <c r="W48" s="59"/>
-      <c r="X48" s="59"/>
-      <c r="Y48" s="59"/>
-      <c r="Z48" s="59"/>
-      <c r="AA48" s="59"/>
-      <c r="AB48" s="59"/>
-      <c r="AC48" s="59"/>
-      <c r="AD48" s="59"/>
-      <c r="AE48" s="59"/>
-      <c r="AF48" s="59"/>
+      <c r="J48" s="67"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
+      <c r="M48" s="67"/>
+      <c r="N48" s="67"/>
+      <c r="O48" s="67"/>
+      <c r="P48" s="67"/>
+      <c r="Q48" s="67"/>
+      <c r="R48" s="67"/>
+      <c r="S48" s="67"/>
+      <c r="T48" s="68"/>
+      <c r="U48" s="73"/>
+      <c r="V48" s="74"/>
+      <c r="W48" s="74"/>
+      <c r="X48" s="74"/>
+      <c r="Y48" s="74"/>
+      <c r="Z48" s="74"/>
+      <c r="AA48" s="74"/>
+      <c r="AB48" s="74"/>
+      <c r="AC48" s="74"/>
+      <c r="AD48" s="74"/>
+      <c r="AE48" s="74"/>
+      <c r="AF48" s="74"/>
     </row>
     <row r="49" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="69" t="s">
+      <c r="A49" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="67"/>
-      <c r="C49" s="67"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="44"/>
       <c r="E49" s="49"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="119"/>
-      <c r="I49" s="64" t="s">
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="117"/>
+      <c r="I49" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="J49" s="65"/>
-      <c r="K49" s="65"/>
-      <c r="L49" s="65"/>
-      <c r="M49" s="65"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="70"/>
+      <c r="M49" s="70"/>
       <c r="N49" s="35"/>
-      <c r="O49" s="65" t="s">
+      <c r="O49" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="P49" s="65"/>
-      <c r="Q49" s="65"/>
-      <c r="R49" s="65"/>
-      <c r="S49" s="65"/>
+      <c r="P49" s="70"/>
+      <c r="Q49" s="70"/>
+      <c r="R49" s="70"/>
+      <c r="S49" s="70"/>
       <c r="T49" s="34"/>
-      <c r="U49" s="58"/>
-      <c r="V49" s="59"/>
-      <c r="W49" s="59"/>
-      <c r="X49" s="59"/>
-      <c r="Y49" s="59"/>
-      <c r="Z49" s="59"/>
-      <c r="AA49" s="59"/>
-      <c r="AB49" s="59"/>
-      <c r="AC49" s="59"/>
-      <c r="AD49" s="59"/>
-      <c r="AE49" s="59"/>
-      <c r="AF49" s="59"/>
+      <c r="U49" s="73"/>
+      <c r="V49" s="74"/>
+      <c r="W49" s="74"/>
+      <c r="X49" s="74"/>
+      <c r="Y49" s="74"/>
+      <c r="Z49" s="74"/>
+      <c r="AA49" s="74"/>
+      <c r="AB49" s="74"/>
+      <c r="AC49" s="74"/>
+      <c r="AD49" s="74"/>
+      <c r="AE49" s="74"/>
+      <c r="AF49" s="74"/>
     </row>
     <row r="50" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="67"/>
-      <c r="C50" s="67"/>
+      <c r="B50" s="58"/>
+      <c r="C50" s="58"/>
       <c r="D50" s="44"/>
       <c r="E50" s="49"/>
-      <c r="F50" s="131"/>
-      <c r="G50" s="131"/>
-      <c r="H50" s="132"/>
+      <c r="F50" s="129"/>
+      <c r="G50" s="129"/>
+      <c r="H50" s="130"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
       <c r="K50" s="14"/>
@@ -3447,25 +3336,25 @@
       <c r="R50" s="14"/>
       <c r="S50" s="14"/>
       <c r="T50" s="15"/>
-      <c r="U50" s="58"/>
-      <c r="V50" s="59"/>
-      <c r="W50" s="59"/>
-      <c r="X50" s="59"/>
-      <c r="Y50" s="59"/>
-      <c r="Z50" s="59"/>
-      <c r="AA50" s="59"/>
-      <c r="AB50" s="59"/>
-      <c r="AC50" s="59"/>
-      <c r="AD50" s="59"/>
-      <c r="AE50" s="59"/>
-      <c r="AF50" s="59"/>
+      <c r="U50" s="73"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="74"/>
+      <c r="X50" s="74"/>
+      <c r="Y50" s="74"/>
+      <c r="Z50" s="74"/>
+      <c r="AA50" s="74"/>
+      <c r="AB50" s="74"/>
+      <c r="AC50" s="74"/>
+      <c r="AD50" s="74"/>
+      <c r="AE50" s="74"/>
+      <c r="AF50" s="74"/>
     </row>
     <row r="51" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="67"/>
-      <c r="C51" s="67"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="58"/>
       <c r="D51" s="44"/>
       <c r="E51" s="49"/>
       <c r="F51" s="50"/>
@@ -3483,29 +3372,29 @@
       <c r="R51" s="16"/>
       <c r="S51" s="16"/>
       <c r="T51" s="23"/>
-      <c r="U51" s="60"/>
-      <c r="V51" s="61"/>
-      <c r="W51" s="61"/>
-      <c r="X51" s="61"/>
-      <c r="Y51" s="61"/>
-      <c r="Z51" s="61"/>
-      <c r="AA51" s="61"/>
-      <c r="AB51" s="61"/>
-      <c r="AC51" s="61"/>
-      <c r="AD51" s="61"/>
-      <c r="AE51" s="61"/>
-      <c r="AF51" s="61"/>
+      <c r="U51" s="75"/>
+      <c r="V51" s="76"/>
+      <c r="W51" s="76"/>
+      <c r="X51" s="76"/>
+      <c r="Y51" s="76"/>
+      <c r="Z51" s="76"/>
+      <c r="AA51" s="76"/>
+      <c r="AB51" s="76"/>
+      <c r="AC51" s="76"/>
+      <c r="AD51" s="76"/>
+      <c r="AE51" s="76"/>
+      <c r="AF51" s="76"/>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A52" s="73" t="s">
+      <c r="A52" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="67"/>
-      <c r="C52" s="67"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
+      <c r="B52" s="58"/>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="58"/>
+      <c r="F52" s="58"/>
+      <c r="G52" s="58"/>
       <c r="H52" s="11"/>
       <c r="I52" s="16"/>
       <c r="J52" s="16"/>
@@ -3521,16 +3410,16 @@
       <c r="T52" s="23"/>
     </row>
     <row r="53" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="69" t="s">
+      <c r="A53" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="B53" s="67"/>
-      <c r="C53" s="67"/>
+      <c r="B53" s="58"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="44"/>
       <c r="E53" s="49"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="67"/>
-      <c r="H53" s="119"/>
+      <c r="F53" s="58"/>
+      <c r="G53" s="58"/>
+      <c r="H53" s="117"/>
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
       <c r="K53" s="13"/>
@@ -3543,150 +3432,150 @@
       <c r="R53" s="13"/>
       <c r="S53" s="13"/>
       <c r="T53" s="2"/>
-      <c r="U53" s="91" t="s">
+      <c r="U53" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="V53" s="92"/>
-      <c r="W53" s="92"/>
-      <c r="X53" s="92"/>
-      <c r="Y53" s="92"/>
-      <c r="Z53" s="92"/>
-      <c r="AA53" s="92"/>
-      <c r="AB53" s="92"/>
-      <c r="AC53" s="92"/>
-      <c r="AD53" s="92"/>
-      <c r="AE53" s="92"/>
-      <c r="AF53" s="92"/>
+      <c r="V53" s="93"/>
+      <c r="W53" s="93"/>
+      <c r="X53" s="93"/>
+      <c r="Y53" s="93"/>
+      <c r="Z53" s="93"/>
+      <c r="AA53" s="93"/>
+      <c r="AB53" s="93"/>
+      <c r="AC53" s="93"/>
+      <c r="AD53" s="93"/>
+      <c r="AE53" s="93"/>
+      <c r="AF53" s="93"/>
     </row>
     <row r="54" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B54" s="67"/>
-      <c r="C54" s="67"/>
+      <c r="B54" s="58"/>
+      <c r="C54" s="58"/>
       <c r="D54" s="44"/>
       <c r="E54" s="49"/>
-      <c r="F54" s="131"/>
-      <c r="G54" s="131"/>
-      <c r="H54" s="132"/>
-      <c r="I54" s="62" t="s">
+      <c r="F54" s="129"/>
+      <c r="G54" s="129"/>
+      <c r="H54" s="130"/>
+      <c r="I54" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="J54" s="63"/>
-      <c r="K54" s="63"/>
-      <c r="L54" s="63"/>
-      <c r="M54" s="63"/>
-      <c r="N54" s="63"/>
-      <c r="O54" s="63"/>
-      <c r="P54" s="63"/>
-      <c r="Q54" s="63"/>
-      <c r="R54" s="63"/>
-      <c r="S54" s="63"/>
-      <c r="T54" s="77"/>
-      <c r="U54" s="90" t="s">
+      <c r="J54" s="67"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="67"/>
+      <c r="M54" s="67"/>
+      <c r="N54" s="67"/>
+      <c r="O54" s="67"/>
+      <c r="P54" s="67"/>
+      <c r="Q54" s="67"/>
+      <c r="R54" s="67"/>
+      <c r="S54" s="67"/>
+      <c r="T54" s="68"/>
+      <c r="U54" s="91" t="s">
         <v>131</v>
       </c>
-      <c r="V54" s="85"/>
-      <c r="W54" s="85"/>
-      <c r="X54" s="85"/>
-      <c r="Y54" s="85"/>
-      <c r="Z54" s="85"/>
-      <c r="AA54" s="85"/>
-      <c r="AB54" s="85"/>
-      <c r="AC54" s="85"/>
-      <c r="AD54" s="85"/>
-      <c r="AE54" s="85"/>
-      <c r="AF54" s="85"/>
+      <c r="V54" s="86"/>
+      <c r="W54" s="86"/>
+      <c r="X54" s="86"/>
+      <c r="Y54" s="86"/>
+      <c r="Z54" s="86"/>
+      <c r="AA54" s="86"/>
+      <c r="AB54" s="86"/>
+      <c r="AC54" s="86"/>
+      <c r="AD54" s="86"/>
+      <c r="AE54" s="86"/>
+      <c r="AF54" s="86"/>
     </row>
     <row r="55" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B55" s="67"/>
-      <c r="C55" s="67"/>
+      <c r="B55" s="58"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="44"/>
       <c r="E55" s="49"/>
       <c r="F55" s="50"/>
       <c r="G55" s="50"/>
       <c r="H55" s="23"/>
-      <c r="I55" s="62" t="s">
+      <c r="I55" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="J55" s="63"/>
-      <c r="K55" s="63"/>
-      <c r="L55" s="63"/>
-      <c r="M55" s="63"/>
-      <c r="N55" s="63"/>
-      <c r="O55" s="63"/>
-      <c r="P55" s="63"/>
-      <c r="Q55" s="63"/>
-      <c r="R55" s="63"/>
-      <c r="S55" s="63"/>
-      <c r="T55" s="77"/>
-      <c r="U55" s="90"/>
-      <c r="V55" s="85"/>
-      <c r="W55" s="85"/>
-      <c r="X55" s="85"/>
-      <c r="Y55" s="85"/>
-      <c r="Z55" s="85"/>
-      <c r="AA55" s="85"/>
-      <c r="AB55" s="85"/>
-      <c r="AC55" s="85"/>
-      <c r="AD55" s="85"/>
-      <c r="AE55" s="85"/>
-      <c r="AF55" s="85"/>
+      <c r="J55" s="67"/>
+      <c r="K55" s="67"/>
+      <c r="L55" s="67"/>
+      <c r="M55" s="67"/>
+      <c r="N55" s="67"/>
+      <c r="O55" s="67"/>
+      <c r="P55" s="67"/>
+      <c r="Q55" s="67"/>
+      <c r="R55" s="67"/>
+      <c r="S55" s="67"/>
+      <c r="T55" s="68"/>
+      <c r="U55" s="91"/>
+      <c r="V55" s="86"/>
+      <c r="W55" s="86"/>
+      <c r="X55" s="86"/>
+      <c r="Y55" s="86"/>
+      <c r="Z55" s="86"/>
+      <c r="AA55" s="86"/>
+      <c r="AB55" s="86"/>
+      <c r="AC55" s="86"/>
+      <c r="AD55" s="86"/>
+      <c r="AE55" s="86"/>
+      <c r="AF55" s="86"/>
     </row>
     <row r="56" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="73" t="s">
+      <c r="A56" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="67"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="67"/>
-      <c r="E56" s="67"/>
-      <c r="F56" s="67"/>
-      <c r="G56" s="67"/>
+      <c r="B56" s="58"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
       <c r="H56" s="11"/>
-      <c r="I56" s="64" t="s">
+      <c r="I56" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="J56" s="65"/>
-      <c r="K56" s="65"/>
+      <c r="J56" s="70"/>
+      <c r="K56" s="70"/>
       <c r="L56" s="33"/>
-      <c r="M56" s="65" t="s">
+      <c r="M56" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="N56" s="65"/>
-      <c r="O56" s="65"/>
-      <c r="P56" s="65"/>
-      <c r="Q56" s="65"/>
-      <c r="R56" s="55"/>
-      <c r="S56" s="55"/>
-      <c r="T56" s="57"/>
-      <c r="U56" s="90"/>
-      <c r="V56" s="85"/>
-      <c r="W56" s="85"/>
-      <c r="X56" s="85"/>
-      <c r="Y56" s="85"/>
-      <c r="Z56" s="85"/>
-      <c r="AA56" s="85"/>
-      <c r="AB56" s="85"/>
-      <c r="AC56" s="85"/>
-      <c r="AD56" s="85"/>
-      <c r="AE56" s="85"/>
-      <c r="AF56" s="85"/>
+      <c r="N56" s="70"/>
+      <c r="O56" s="70"/>
+      <c r="P56" s="70"/>
+      <c r="Q56" s="70"/>
+      <c r="R56" s="77"/>
+      <c r="S56" s="77"/>
+      <c r="T56" s="96"/>
+      <c r="U56" s="91"/>
+      <c r="V56" s="86"/>
+      <c r="W56" s="86"/>
+      <c r="X56" s="86"/>
+      <c r="Y56" s="86"/>
+      <c r="Z56" s="86"/>
+      <c r="AA56" s="86"/>
+      <c r="AB56" s="86"/>
+      <c r="AC56" s="86"/>
+      <c r="AD56" s="86"/>
+      <c r="AE56" s="86"/>
+      <c r="AF56" s="86"/>
     </row>
     <row r="57" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="B57" s="67"/>
-      <c r="C57" s="67"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
       <c r="D57" s="44"/>
       <c r="E57" s="49"/>
-      <c r="F57" s="67"/>
-      <c r="G57" s="67"/>
-      <c r="H57" s="119"/>
+      <c r="F57" s="58"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="117"/>
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
       <c r="K57" s="13"/>
@@ -3695,105 +3584,105 @@
       <c r="N57" s="13"/>
       <c r="O57" s="13"/>
       <c r="P57" s="13"/>
-      <c r="Q57" s="71" t="s">
+      <c r="Q57" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="R57" s="71"/>
-      <c r="S57" s="71"/>
-      <c r="T57" s="72"/>
-      <c r="U57" s="90"/>
-      <c r="V57" s="85"/>
-      <c r="W57" s="85"/>
-      <c r="X57" s="85"/>
-      <c r="Y57" s="85"/>
-      <c r="Z57" s="85"/>
-      <c r="AA57" s="85"/>
-      <c r="AB57" s="85"/>
-      <c r="AC57" s="85"/>
-      <c r="AD57" s="85"/>
-      <c r="AE57" s="85"/>
-      <c r="AF57" s="85"/>
+      <c r="R57" s="60"/>
+      <c r="S57" s="60"/>
+      <c r="T57" s="61"/>
+      <c r="U57" s="91"/>
+      <c r="V57" s="86"/>
+      <c r="W57" s="86"/>
+      <c r="X57" s="86"/>
+      <c r="Y57" s="86"/>
+      <c r="Z57" s="86"/>
+      <c r="AA57" s="86"/>
+      <c r="AB57" s="86"/>
+      <c r="AC57" s="86"/>
+      <c r="AD57" s="86"/>
+      <c r="AE57" s="86"/>
+      <c r="AF57" s="86"/>
     </row>
     <row r="58" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B58" s="67"/>
-      <c r="C58" s="67"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="44"/>
       <c r="E58" s="49"/>
-      <c r="F58" s="131"/>
-      <c r="G58" s="131"/>
-      <c r="H58" s="132"/>
-      <c r="I58" s="62" t="s">
+      <c r="F58" s="129"/>
+      <c r="G58" s="129"/>
+      <c r="H58" s="130"/>
+      <c r="I58" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="J58" s="63"/>
-      <c r="K58" s="63"/>
-      <c r="L58" s="63"/>
-      <c r="M58" s="63"/>
-      <c r="N58" s="63"/>
-      <c r="O58" s="63"/>
-      <c r="P58" s="63"/>
-      <c r="Q58" s="63"/>
-      <c r="R58" s="63"/>
-      <c r="S58" s="63"/>
-      <c r="T58" s="77"/>
+      <c r="J58" s="67"/>
+      <c r="K58" s="67"/>
+      <c r="L58" s="67"/>
+      <c r="M58" s="67"/>
+      <c r="N58" s="67"/>
+      <c r="O58" s="67"/>
+      <c r="P58" s="67"/>
+      <c r="Q58" s="67"/>
+      <c r="R58" s="67"/>
+      <c r="S58" s="67"/>
+      <c r="T58" s="68"/>
       <c r="U58" s="1"/>
       <c r="AF58" s="13"/>
     </row>
     <row r="59" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="67"/>
-      <c r="C59" s="67"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="58"/>
       <c r="D59" s="44"/>
       <c r="E59" s="49"/>
       <c r="F59" s="50"/>
       <c r="G59" s="50"/>
       <c r="H59" s="23"/>
-      <c r="I59" s="96" t="s">
+      <c r="I59" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="J59" s="97"/>
-      <c r="K59" s="97"/>
+      <c r="J59" s="77"/>
+      <c r="K59" s="77"/>
       <c r="L59" s="33"/>
-      <c r="M59" s="65" t="s">
+      <c r="M59" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="N59" s="65"/>
-      <c r="O59" s="65"/>
-      <c r="P59" s="65"/>
-      <c r="Q59" s="65"/>
-      <c r="R59" s="55"/>
-      <c r="S59" s="55"/>
-      <c r="T59" s="57"/>
+      <c r="N59" s="70"/>
+      <c r="O59" s="70"/>
+      <c r="P59" s="70"/>
+      <c r="Q59" s="70"/>
+      <c r="R59" s="77"/>
+      <c r="S59" s="77"/>
+      <c r="T59" s="96"/>
       <c r="U59" s="1"/>
-      <c r="V59" s="81" t="s">
+      <c r="V59" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="W59" s="82"/>
-      <c r="X59" s="82"/>
-      <c r="Y59" s="82"/>
-      <c r="Z59" s="82"/>
-      <c r="AA59" s="82"/>
-      <c r="AB59" s="82"/>
-      <c r="AC59" s="82"/>
-      <c r="AD59" s="82"/>
-      <c r="AE59" s="83"/>
+      <c r="W59" s="83"/>
+      <c r="X59" s="83"/>
+      <c r="Y59" s="83"/>
+      <c r="Z59" s="83"/>
+      <c r="AA59" s="83"/>
+      <c r="AB59" s="83"/>
+      <c r="AC59" s="83"/>
+      <c r="AD59" s="83"/>
+      <c r="AE59" s="84"/>
       <c r="AF59" s="13"/>
     </row>
     <row r="60" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="73" t="s">
+      <c r="A60" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B60" s="67"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="67"/>
-      <c r="E60" s="67"/>
-      <c r="F60" s="67"/>
-      <c r="G60" s="67"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
       <c r="H60" s="11"/>
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
@@ -3803,171 +3692,171 @@
       <c r="N60" s="13"/>
       <c r="O60" s="13"/>
       <c r="P60" s="13"/>
-      <c r="Q60" s="71" t="s">
+      <c r="Q60" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="R60" s="71"/>
-      <c r="S60" s="71"/>
-      <c r="T60" s="72"/>
+      <c r="R60" s="60"/>
+      <c r="S60" s="60"/>
+      <c r="T60" s="61"/>
       <c r="U60" s="1"/>
-      <c r="V60" s="84"/>
-      <c r="W60" s="85"/>
-      <c r="X60" s="85"/>
-      <c r="Y60" s="85"/>
-      <c r="Z60" s="85"/>
-      <c r="AA60" s="85"/>
-      <c r="AB60" s="85"/>
-      <c r="AC60" s="85"/>
-      <c r="AD60" s="85"/>
-      <c r="AE60" s="86"/>
+      <c r="V60" s="85"/>
+      <c r="W60" s="86"/>
+      <c r="X60" s="86"/>
+      <c r="Y60" s="86"/>
+      <c r="Z60" s="86"/>
+      <c r="AA60" s="86"/>
+      <c r="AB60" s="86"/>
+      <c r="AC60" s="86"/>
+      <c r="AD60" s="86"/>
+      <c r="AE60" s="87"/>
       <c r="AF60" s="13"/>
     </row>
     <row r="61" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="69" t="s">
+      <c r="A61" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="B61" s="67"/>
-      <c r="C61" s="67"/>
+      <c r="B61" s="58"/>
+      <c r="C61" s="58"/>
       <c r="D61" s="44"/>
       <c r="E61" s="49"/>
-      <c r="F61" s="67"/>
-      <c r="G61" s="67"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="62" t="s">
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="117"/>
+      <c r="I61" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63"/>
-      <c r="L61" s="63"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="63"/>
-      <c r="O61" s="63"/>
-      <c r="P61" s="63"/>
-      <c r="Q61" s="63"/>
-      <c r="R61" s="63"/>
-      <c r="S61" s="63"/>
-      <c r="T61" s="77"/>
+      <c r="J61" s="67"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="67"/>
+      <c r="M61" s="67"/>
+      <c r="N61" s="67"/>
+      <c r="O61" s="67"/>
+      <c r="P61" s="67"/>
+      <c r="Q61" s="67"/>
+      <c r="R61" s="67"/>
+      <c r="S61" s="67"/>
+      <c r="T61" s="68"/>
       <c r="U61" s="1"/>
-      <c r="V61" s="84"/>
-      <c r="W61" s="85"/>
-      <c r="X61" s="85"/>
-      <c r="Y61" s="85"/>
-      <c r="Z61" s="85"/>
-      <c r="AA61" s="85"/>
-      <c r="AB61" s="85"/>
-      <c r="AC61" s="85"/>
-      <c r="AD61" s="85"/>
-      <c r="AE61" s="86"/>
+      <c r="V61" s="85"/>
+      <c r="W61" s="86"/>
+      <c r="X61" s="86"/>
+      <c r="Y61" s="86"/>
+      <c r="Z61" s="86"/>
+      <c r="AA61" s="86"/>
+      <c r="AB61" s="86"/>
+      <c r="AC61" s="86"/>
+      <c r="AD61" s="86"/>
+      <c r="AE61" s="87"/>
       <c r="AF61" s="13"/>
     </row>
     <row r="62" spans="1:32" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="69" t="s">
+      <c r="A62" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B62" s="67"/>
-      <c r="C62" s="67"/>
+      <c r="B62" s="58"/>
+      <c r="C62" s="58"/>
       <c r="D62" s="44"/>
       <c r="E62" s="49"/>
-      <c r="F62" s="131"/>
-      <c r="G62" s="131"/>
-      <c r="H62" s="132"/>
-      <c r="I62" s="64" t="s">
+      <c r="F62" s="129"/>
+      <c r="G62" s="129"/>
+      <c r="H62" s="130"/>
+      <c r="I62" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="J62" s="95"/>
-      <c r="K62" s="95"/>
+      <c r="J62" s="97"/>
+      <c r="K62" s="97"/>
       <c r="L62" s="33"/>
-      <c r="M62" s="65" t="s">
+      <c r="M62" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="N62" s="65"/>
-      <c r="O62" s="65"/>
+      <c r="N62" s="70"/>
+      <c r="O62" s="70"/>
       <c r="P62" s="33"/>
-      <c r="Q62" s="65" t="s">
+      <c r="Q62" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="R62" s="65"/>
-      <c r="S62" s="65"/>
+      <c r="R62" s="70"/>
+      <c r="S62" s="70"/>
       <c r="T62" s="34"/>
       <c r="U62" s="1"/>
-      <c r="V62" s="84"/>
-      <c r="W62" s="85"/>
-      <c r="X62" s="85"/>
-      <c r="Y62" s="85"/>
-      <c r="Z62" s="85"/>
-      <c r="AA62" s="85"/>
-      <c r="AB62" s="85"/>
-      <c r="AC62" s="85"/>
-      <c r="AD62" s="85"/>
-      <c r="AE62" s="86"/>
+      <c r="V62" s="85"/>
+      <c r="W62" s="86"/>
+      <c r="X62" s="86"/>
+      <c r="Y62" s="86"/>
+      <c r="Z62" s="86"/>
+      <c r="AA62" s="86"/>
+      <c r="AB62" s="86"/>
+      <c r="AC62" s="86"/>
+      <c r="AD62" s="86"/>
+      <c r="AE62" s="87"/>
       <c r="AF62" s="13"/>
     </row>
     <row r="63" spans="1:32" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="69" t="s">
+      <c r="A63" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="67"/>
-      <c r="C63" s="67"/>
+      <c r="B63" s="58"/>
+      <c r="C63" s="58"/>
       <c r="D63" s="44"/>
       <c r="E63" s="49"/>
       <c r="F63" s="50"/>
       <c r="G63" s="50"/>
       <c r="H63" s="23"/>
-      <c r="I63" s="62" t="s">
+      <c r="I63" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="J63" s="63"/>
-      <c r="K63" s="63"/>
-      <c r="L63" s="63"/>
-      <c r="M63" s="63"/>
-      <c r="N63" s="63"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="63"/>
-      <c r="Q63" s="63"/>
-      <c r="R63" s="63"/>
-      <c r="S63" s="63"/>
-      <c r="T63" s="77"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="67"/>
+      <c r="M63" s="67"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="67"/>
+      <c r="P63" s="67"/>
+      <c r="Q63" s="67"/>
+      <c r="R63" s="67"/>
+      <c r="S63" s="67"/>
+      <c r="T63" s="68"/>
       <c r="U63" s="1"/>
-      <c r="V63" s="87"/>
-      <c r="W63" s="88"/>
-      <c r="X63" s="88"/>
-      <c r="Y63" s="88"/>
-      <c r="Z63" s="88"/>
-      <c r="AA63" s="88"/>
-      <c r="AB63" s="88"/>
-      <c r="AC63" s="88"/>
-      <c r="AD63" s="88"/>
-      <c r="AE63" s="89"/>
+      <c r="V63" s="88"/>
+      <c r="W63" s="89"/>
+      <c r="X63" s="89"/>
+      <c r="Y63" s="89"/>
+      <c r="Z63" s="89"/>
+      <c r="AA63" s="89"/>
+      <c r="AB63" s="89"/>
+      <c r="AC63" s="89"/>
+      <c r="AD63" s="89"/>
+      <c r="AE63" s="90"/>
       <c r="AF63" s="13"/>
     </row>
     <row r="64" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="73" t="s">
+      <c r="A64" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="B64" s="67"/>
-      <c r="C64" s="67"/>
-      <c r="D64" s="67"/>
-      <c r="E64" s="67"/>
-      <c r="F64" s="67"/>
-      <c r="G64" s="67"/>
+      <c r="B64" s="58"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="58"/>
+      <c r="G64" s="58"/>
       <c r="H64" s="11"/>
-      <c r="I64" s="64" t="s">
+      <c r="I64" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="J64" s="95"/>
-      <c r="K64" s="95"/>
+      <c r="J64" s="97"/>
+      <c r="K64" s="97"/>
       <c r="L64" s="33"/>
-      <c r="M64" s="65" t="s">
+      <c r="M64" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="N64" s="65"/>
-      <c r="O64" s="65"/>
+      <c r="N64" s="70"/>
+      <c r="O64" s="70"/>
       <c r="P64" s="33"/>
-      <c r="Q64" s="65" t="s">
+      <c r="Q64" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="R64" s="65"/>
-      <c r="S64" s="65"/>
+      <c r="R64" s="70"/>
+      <c r="S64" s="70"/>
       <c r="T64" s="34"/>
       <c r="U64" s="1"/>
       <c r="V64" s="20"/>
@@ -3981,16 +3870,16 @@
       <c r="AD64" s="1"/>
     </row>
     <row r="65" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="69" t="s">
+      <c r="A65" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="67"/>
-      <c r="C65" s="67"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="58"/>
       <c r="D65" s="45"/>
       <c r="E65" s="52"/>
-      <c r="F65" s="129"/>
-      <c r="G65" s="129"/>
-      <c r="H65" s="130"/>
+      <c r="F65" s="127"/>
+      <c r="G65" s="127"/>
+      <c r="H65" s="128"/>
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
       <c r="K65" s="13"/>
@@ -4004,30 +3893,30 @@
       <c r="S65" s="13"/>
       <c r="T65" s="2"/>
       <c r="U65" s="1"/>
-      <c r="V65" s="120" t="s">
+      <c r="V65" s="118" t="s">
         <v>133</v>
       </c>
-      <c r="W65" s="121"/>
-      <c r="X65" s="121"/>
-      <c r="Y65" s="121"/>
-      <c r="Z65" s="121"/>
-      <c r="AA65" s="121"/>
-      <c r="AB65" s="121"/>
-      <c r="AC65" s="121"/>
-      <c r="AD65" s="121"/>
-      <c r="AE65" s="122"/>
+      <c r="W65" s="119"/>
+      <c r="X65" s="119"/>
+      <c r="Y65" s="119"/>
+      <c r="Z65" s="119"/>
+      <c r="AA65" s="119"/>
+      <c r="AB65" s="119"/>
+      <c r="AC65" s="119"/>
+      <c r="AD65" s="119"/>
+      <c r="AE65" s="120"/>
     </row>
     <row r="66" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="69" t="s">
+      <c r="A66" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="B66" s="67"/>
-      <c r="C66" s="67"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="58"/>
       <c r="D66" s="45"/>
       <c r="E66" s="52"/>
-      <c r="F66" s="133"/>
-      <c r="G66" s="133"/>
-      <c r="H66" s="134"/>
+      <c r="F66" s="131"/>
+      <c r="G66" s="131"/>
+      <c r="H66" s="132"/>
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
       <c r="K66" s="13"/>
@@ -4041,23 +3930,23 @@
       <c r="S66" s="13"/>
       <c r="T66" s="26"/>
       <c r="U66" s="1"/>
-      <c r="V66" s="123"/>
-      <c r="W66" s="124"/>
-      <c r="X66" s="124"/>
-      <c r="Y66" s="124"/>
-      <c r="Z66" s="124"/>
-      <c r="AA66" s="124"/>
-      <c r="AB66" s="124"/>
-      <c r="AC66" s="124"/>
-      <c r="AD66" s="124"/>
-      <c r="AE66" s="125"/>
+      <c r="V66" s="121"/>
+      <c r="W66" s="122"/>
+      <c r="X66" s="122"/>
+      <c r="Y66" s="122"/>
+      <c r="Z66" s="122"/>
+      <c r="AA66" s="122"/>
+      <c r="AB66" s="122"/>
+      <c r="AC66" s="122"/>
+      <c r="AD66" s="122"/>
+      <c r="AE66" s="123"/>
     </row>
     <row r="67" spans="1:33" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="69" t="s">
+      <c r="A67" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="58"/>
       <c r="D67" s="45"/>
       <c r="E67" s="52"/>
       <c r="F67" s="53"/>
@@ -4076,16 +3965,16 @@
       <c r="S67" s="13"/>
       <c r="T67" s="2"/>
       <c r="U67" s="1"/>
-      <c r="V67" s="126"/>
-      <c r="W67" s="127"/>
-      <c r="X67" s="127"/>
-      <c r="Y67" s="127"/>
-      <c r="Z67" s="127"/>
-      <c r="AA67" s="127"/>
-      <c r="AB67" s="127"/>
-      <c r="AC67" s="127"/>
-      <c r="AD67" s="127"/>
-      <c r="AE67" s="128"/>
+      <c r="V67" s="124"/>
+      <c r="W67" s="125"/>
+      <c r="X67" s="125"/>
+      <c r="Y67" s="125"/>
+      <c r="Z67" s="125"/>
+      <c r="AA67" s="125"/>
+      <c r="AB67" s="125"/>
+      <c r="AC67" s="125"/>
+      <c r="AD67" s="125"/>
+      <c r="AE67" s="126"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="10"/>
@@ -4123,7 +4012,7 @@
       <c r="AG68" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="166">
+  <mergeCells count="171">
     <mergeCell ref="V65:AE67"/>
     <mergeCell ref="A67:C67"/>
     <mergeCell ref="A62:C62"/>
@@ -4171,8 +4060,6 @@
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="A29:H29"/>
     <mergeCell ref="A30:H30"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="U22:W22"/>
     <mergeCell ref="Y22:AC22"/>
@@ -4211,6 +4098,9 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="AD22:AF22"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="I36:K36"/>
     <mergeCell ref="M36:O36"/>
     <mergeCell ref="Q36:S36"/>
@@ -4232,6 +4122,10 @@
     <mergeCell ref="U29:W29"/>
     <mergeCell ref="AD29:AE29"/>
     <mergeCell ref="I35:T35"/>
+    <mergeCell ref="AC31:AE31"/>
+    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="I31:T31"/>
+    <mergeCell ref="R56:T56"/>
     <mergeCell ref="I64:K64"/>
     <mergeCell ref="M62:O62"/>
     <mergeCell ref="M64:O64"/>
@@ -4242,8 +4136,14 @@
     <mergeCell ref="Q60:T60"/>
     <mergeCell ref="M59:Q59"/>
     <mergeCell ref="I59:K59"/>
-    <mergeCell ref="AC31:AE31"/>
-    <mergeCell ref="Y31:AA31"/>
+    <mergeCell ref="O32:S32"/>
+    <mergeCell ref="I33:T33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="U24:AF24"/>
+    <mergeCell ref="I30:M30"/>
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="V59:AE63"/>
     <mergeCell ref="U54:AF57"/>
     <mergeCell ref="U53:AF53"/>
@@ -4259,16 +4159,7 @@
     <mergeCell ref="I46:T46"/>
     <mergeCell ref="I48:T48"/>
     <mergeCell ref="I41:T41"/>
-    <mergeCell ref="I31:T31"/>
-    <mergeCell ref="I32:M32"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="I33:T33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="U24:AF24"/>
-    <mergeCell ref="I30:M30"/>
-    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="R59:T59"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="A46:C46"/>
     <mergeCell ref="A47:H47"/>
@@ -4290,6 +4181,9 @@
     <mergeCell ref="AA36:AE36"/>
     <mergeCell ref="U38:AC38"/>
     <mergeCell ref="U37:AE37"/>
+    <mergeCell ref="U45:AF51"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="I32:M32"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>

</xml_diff>